<commit_message>
Add moon to code
</commit_message>
<xml_diff>
--- a/Masses astres.xlsx
+++ b/Masses astres.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bc217c0b68332ccc/Bureau/python/Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{1EFD99F7-708A-4457-A218-EB357170E642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D91CC694-709A-4265-9D31-91173C4058BB}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{1EFD99F7-708A-4457-A218-EB357170E642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5E9D7C1-F072-4D34-84FC-652B0928B418}"/>
   <bookViews>
     <workbookView xWindow="1605" yWindow="1530" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
   <si>
     <t>Astres</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>paramètre orienter planète</t>
+  </si>
+  <si>
+    <t>Lune</t>
   </si>
 </sst>
 </file>
@@ -270,7 +273,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -324,12 +327,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -350,19 +347,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -490,6 +474,19 @@
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -710,22 +707,22 @@
     <tableColumn id="7" xr3:uid="{7B87A2BE-ADED-4EC7-90F4-82312C153D69}" name="vitesse rotation équateur (rad/ds)" dataDxfId="11">
       <calculatedColumnFormula>DEGREES((F2*1000/3600)/(C2*1000/2))/10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{2C9717ED-55F0-43A9-8BF0-C1A01A73941C}" name="paramètre orienter planète" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{2C9717ED-55F0-43A9-8BF0-C1A01A73941C}" name="paramètre orienter planète" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6B08AFF7-E6AC-487E-A862-54025ABD7D5C}" name="Tableau24" displayName="Tableau24" ref="A19:F33" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6B08AFF7-E6AC-487E-A862-54025ABD7D5C}" name="Tableau24" displayName="Tableau24" ref="A19:F33" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6">
   <autoFilter ref="A19:F33" xr:uid="{6B08AFF7-E6AC-487E-A862-54025ABD7D5C}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{57D8D285-6390-4ADD-8C08-C6E8212288A7}" name="Astres" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{9AA0953F-EB7A-4A32-8A2C-59A3B7D54DD6}" name="Masse" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{42C928A3-CDC0-401D-BBEB-DBDE9C296C9E}" name="Diamètre" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{F3774F47-11B7-41CC-BD67-B0851461EE8E}" name="Aplatissement" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{B4AE3617-38DD-4C16-A173-5946879F54C9}" name="Distance soleil" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{C1001996-59B6-404E-967B-839EFC3F25BB}" name="vitesse rotation équateur (km/h)" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{57D8D285-6390-4ADD-8C08-C6E8212288A7}" name="Astres" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{9AA0953F-EB7A-4A32-8A2C-59A3B7D54DD6}" name="Masse" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{42C928A3-CDC0-401D-BBEB-DBDE9C296C9E}" name="Diamètre" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{F3774F47-11B7-41CC-BD67-B0851461EE8E}" name="Aplatissement" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{B4AE3617-38DD-4C16-A173-5946879F54C9}" name="Distance soleil" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{C1001996-59B6-404E-967B-839EFC3F25BB}" name="vitesse rotation équateur (km/h)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -997,7 +994,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,7 +1030,7 @@
       <c r="G1" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="18" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1061,7 +1058,7 @@
         <f t="shared" ref="G2:G10" si="2">DEGREES((F2*1000/3600)/(C2*1000/2))/10</f>
         <v>3.4055305816646229E-5</v>
       </c>
-      <c r="H2" s="19"/>
+      <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -1086,7 +1083,7 @@
         <f t="shared" si="2"/>
         <v>7.1054459161246225E-3</v>
       </c>
-      <c r="H3" s="19"/>
+      <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
@@ -1111,7 +1108,7 @@
         <f t="shared" si="2"/>
         <v>1.7146803082705271E-6</v>
       </c>
-      <c r="H4" s="19"/>
+      <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
@@ -1137,7 +1134,7 @@
         <f t="shared" si="2"/>
         <v>4.1780743677208288E-4</v>
       </c>
-      <c r="H5" s="19"/>
+      <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
@@ -1162,7 +1159,7 @@
         <f t="shared" si="2"/>
         <v>4.0679178623016831E-4</v>
       </c>
-      <c r="H6" s="19"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
@@ -1187,7 +1184,7 @@
         <f t="shared" si="2"/>
         <v>1.0474457600034644E-3</v>
       </c>
-      <c r="H7" s="19"/>
+      <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
@@ -1212,7 +1209,7 @@
         <f t="shared" si="2"/>
         <v>2.237899480456666E-3</v>
       </c>
-      <c r="H8" s="19"/>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
@@ -1237,7 +1234,7 @@
         <f t="shared" si="2"/>
         <v>5.8035293619330356E-4</v>
       </c>
-      <c r="H9" s="19"/>
+      <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
@@ -1262,7 +1259,7 @@
         <f t="shared" si="2"/>
         <v>6.2083538615236185E-4</v>
       </c>
-      <c r="H10" s="19"/>
+      <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
@@ -1272,17 +1269,19 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="19"/>
+      <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
+      <c r="A12" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="B12" s="5"/>
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
-      <c r="H12" s="19"/>
+      <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
@@ -1292,7 +1291,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
-      <c r="H13" s="19"/>
+      <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
@@ -1302,7 +1301,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="19"/>
+      <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
@@ -1312,7 +1311,7 @@
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="19"/>
+      <c r="H15" s="5"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">

</xml_diff>

<commit_message>
Add angle of all planets
</commit_message>
<xml_diff>
--- a/Masses astres.xlsx
+++ b/Masses astres.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bc217c0b68332ccc/Bureau/python/Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{1EFD99F7-708A-4457-A218-EB357170E642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5E9D7C1-F072-4D34-84FC-652B0928B418}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{1EFD99F7-708A-4457-A218-EB357170E642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADCA5BEF-31C8-4E1E-A6C9-410CE16B7438}"/>
   <bookViews>
-    <workbookView xWindow="1605" yWindow="1530" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t>Astres</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>Lune</t>
+  </si>
+  <si>
+    <t>Angle de rotation (deg)</t>
+  </si>
+  <si>
+    <t>7.23</t>
   </si>
 </sst>
 </file>
@@ -176,7 +182,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -267,13 +273,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFAAAAAA"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFAAAAAA"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFAAAAAA"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -328,6 +347,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -686,6 +708,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -700,7 +726,7 @@
     <tableColumn id="5" xr3:uid="{2859AEC0-DB80-4F8A-8611-2D1CB99408B1}" name="Aplatissement" dataDxfId="14">
       <calculatedColumnFormula>9*10^-6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{FEFB98A5-F681-4A28-8656-83E81E4A53E3}" name="Distance soleil" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{FEFB98A5-F681-4A28-8656-83E81E4A53E3}" name="Angle de rotation (deg)" dataDxfId="13"/>
     <tableColumn id="4" xr3:uid="{F49A900E-B0EE-48B7-858F-35EC2942B732}" name="vitesse rotation équateur (km/h)" dataDxfId="12">
       <calculatedColumnFormula>24*24*60*60</calculatedColumnFormula>
     </tableColumn>
@@ -994,7 +1020,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,7 +1048,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>6</v>
@@ -1049,7 +1075,9 @@
         <f t="shared" ref="D2" si="1">9*10^-6</f>
         <v>9.0000000000000002E-6</v>
       </c>
-      <c r="E2" s="9"/>
+      <c r="E2" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="F2" s="10">
         <f xml:space="preserve">  Tableau2[[#This Row],[Diamètre]]*2*PI()/(24.47*24)</f>
         <v>14900.033453112817</v>
@@ -1075,7 +1103,9 @@
       <c r="D3" s="11">
         <v>0</v>
       </c>
-      <c r="E3" s="10"/>
+      <c r="E3" s="10">
+        <v>0.03</v>
+      </c>
       <c r="F3" s="10">
         <v>10892</v>
       </c>
@@ -1100,7 +1130,9 @@
       <c r="D4" s="11">
         <v>0</v>
       </c>
-      <c r="E4" s="10"/>
+      <c r="E4" s="10">
+        <v>177.36</v>
+      </c>
       <c r="F4" s="10">
         <v>6.52</v>
       </c>
@@ -1126,7 +1158,9 @@
         <f>1/300</f>
         <v>3.3333333333333335E-3</v>
       </c>
-      <c r="E5" s="10"/>
+      <c r="E5" s="10">
+        <v>23.45</v>
+      </c>
       <c r="F5" s="10">
         <v>1674.364</v>
       </c>
@@ -1151,7 +1185,9 @@
       <c r="D6" s="11">
         <v>5.8900000000000003E-3</v>
       </c>
-      <c r="E6" s="10"/>
+      <c r="E6" s="10">
+        <v>25</v>
+      </c>
       <c r="F6" s="10">
         <v>868</v>
       </c>
@@ -1173,10 +1209,12 @@
         <f>71492*2</f>
         <v>142984</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="19">
         <v>6.4869999999999997E-2</v>
       </c>
-      <c r="E7" s="10"/>
+      <c r="E7" s="10">
+        <v>1.304</v>
+      </c>
       <c r="F7" s="10">
         <v>47051</v>
       </c>
@@ -1201,7 +1239,9 @@
       <c r="D8" s="11">
         <v>9.7960000000000005E-2</v>
       </c>
-      <c r="E8" s="13"/>
+      <c r="E8" s="13">
+        <v>27</v>
+      </c>
       <c r="F8" s="11">
         <v>34821</v>
       </c>
@@ -1226,7 +1266,9 @@
       <c r="D9" s="12">
         <v>2.2929999999999999E-2</v>
       </c>
-      <c r="E9" s="10"/>
+      <c r="E9" s="10">
+        <v>98</v>
+      </c>
       <c r="F9" s="11">
         <v>9320</v>
       </c>
@@ -1251,7 +1293,9 @@
       <c r="D10" s="12">
         <v>1.7100000000000001E-2</v>
       </c>
-      <c r="E10" s="10"/>
+      <c r="E10" s="10">
+        <v>28.32</v>
+      </c>
       <c r="F10" s="11">
         <v>9660</v>
       </c>
@@ -1522,9 +1566,10 @@
     <hyperlink ref="A10" r:id="rId19" xr:uid="{9210B17E-554D-4B6F-91E6-8A69109054B9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
   <tableParts count="2">
-    <tablePart r:id="rId20"/>
     <tablePart r:id="rId21"/>
+    <tablePart r:id="rId22"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajout de classe et recuperer des infos du excel
</commit_message>
<xml_diff>
--- a/Masses astres.xlsx
+++ b/Masses astres.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bc217c0b68332ccc/Bureau/python/Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{1EFD99F7-708A-4457-A218-EB357170E642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADCA5BEF-31C8-4E1E-A6C9-410CE16B7438}"/>
+  <xr:revisionPtr revIDLastSave="180" documentId="13_ncr:1_{1EFD99F7-708A-4457-A218-EB357170E642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{908C2DD4-487A-4886-99FE-F815200055F0}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
   <si>
     <t>Astres</t>
   </si>
@@ -99,6 +100,99 @@
   </si>
   <si>
     <t>7.23</t>
+  </si>
+  <si>
+    <t>rotation = (x,y,z)</t>
+  </si>
+  <si>
+    <t>orbit speed = (x,y,z)</t>
+  </si>
+  <si>
+    <t>OrbitRadius</t>
+  </si>
+  <si>
+    <t>rotation speed = [0,0,0]</t>
+  </si>
+  <si>
+    <t>texture</t>
+  </si>
+  <si>
+    <t>'assets/8k_sun'</t>
+  </si>
+  <si>
+    <t>'assets/mercury'</t>
+  </si>
+  <si>
+    <t>'assets/venus1'</t>
+  </si>
+  <si>
+    <t>'assets/mars'</t>
+  </si>
+  <si>
+    <t>'assets/jupiter'</t>
+  </si>
+  <si>
+    <t>'assets/saturn'</t>
+  </si>
+  <si>
+    <t>'assets/uranus'</t>
+  </si>
+  <si>
+    <t>'assets/neptune'</t>
+  </si>
+  <si>
+    <t>(360/365,0,0)</t>
+  </si>
+  <si>
+    <t>[0,-360/24,0]</t>
+  </si>
+  <si>
+    <t>scale</t>
+  </si>
+  <si>
+    <t>3.6704</t>
+  </si>
+  <si>
+    <t>3.5562</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (23.45,0,0)</t>
+  </si>
+  <si>
+    <t>(0.03,0,0)</t>
+  </si>
+  <si>
+    <t>(7.23,0,0)</t>
+  </si>
+  <si>
+    <t>(177.36,0,0)</t>
+  </si>
+  <si>
+    <t>(25,0,0)</t>
+  </si>
+  <si>
+    <t>(1.304,0,0)</t>
+  </si>
+  <si>
+    <t>(27,0,0)</t>
+  </si>
+  <si>
+    <t>(98.32,0,0)</t>
+  </si>
+  <si>
+    <t>(28.32,0,0)</t>
+  </si>
+  <si>
+    <t>assets/earth</t>
+  </si>
+  <si>
+    <t>position x</t>
+  </si>
+  <si>
+    <t>position y</t>
+  </si>
+  <si>
+    <t>position z</t>
   </si>
 </sst>
 </file>
@@ -108,7 +202,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,6 +261,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -182,7 +282,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -286,13 +386,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -351,13 +460,326 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
     <cellStyle name="Milliers" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="40">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -715,40 +1137,68 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{524A4480-6DAB-4CB9-8F9A-6D7582E76A58}" name="Tableau2" displayName="Tableau2" ref="A1:H15" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{524A4480-6DAB-4CB9-8F9A-6D7582E76A58}" name="Tableau2" displayName="Tableau2" ref="A1:H15" totalsRowShown="0" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36">
   <autoFilter ref="A1:H15" xr:uid="{524A4480-6DAB-4CB9-8F9A-6D7582E76A58}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{A3C56C48-4D56-4E78-8EAC-8A8834CCB7B6}" name="Astres" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{0ACD23B6-9D0A-41BC-9D2A-22A123127B9A}" name="Masse" dataDxfId="16">
+    <tableColumn id="1" xr3:uid="{A3C56C48-4D56-4E78-8EAC-8A8834CCB7B6}" name="Astres" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{0ACD23B6-9D0A-41BC-9D2A-22A123127B9A}" name="Masse" dataDxfId="34">
       <calculatedColumnFormula>1.988*10^30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{5449565D-8FF5-4D07-BC9E-A81B7DCC7C09}" name="Diamètre" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{2859AEC0-DB80-4F8A-8611-2D1CB99408B1}" name="Aplatissement" dataDxfId="14">
+    <tableColumn id="3" xr3:uid="{5449565D-8FF5-4D07-BC9E-A81B7DCC7C09}" name="Diamètre" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{2859AEC0-DB80-4F8A-8611-2D1CB99408B1}" name="Aplatissement" dataDxfId="32">
       <calculatedColumnFormula>9*10^-6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{FEFB98A5-F681-4A28-8656-83E81E4A53E3}" name="Angle de rotation (deg)" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{F49A900E-B0EE-48B7-858F-35EC2942B732}" name="vitesse rotation équateur (km/h)" dataDxfId="12">
+    <tableColumn id="6" xr3:uid="{FEFB98A5-F681-4A28-8656-83E81E4A53E3}" name="Angle de rotation (deg)" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{F49A900E-B0EE-48B7-858F-35EC2942B732}" name="vitesse rotation équateur (km/h)" dataDxfId="30">
       <calculatedColumnFormula>24*24*60*60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{7B87A2BE-ADED-4EC7-90F4-82312C153D69}" name="vitesse rotation équateur (rad/ds)" dataDxfId="11">
+    <tableColumn id="7" xr3:uid="{7B87A2BE-ADED-4EC7-90F4-82312C153D69}" name="vitesse rotation équateur (rad/ds)" dataDxfId="29">
       <calculatedColumnFormula>DEGREES((F2*1000/3600)/(C2*1000/2))/10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{2C9717ED-55F0-43A9-8BF0-C1A01A73941C}" name="paramètre orienter planète" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{2C9717ED-55F0-43A9-8BF0-C1A01A73941C}" name="paramètre orienter planète" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6B08AFF7-E6AC-487E-A862-54025ABD7D5C}" name="Tableau24" displayName="Tableau24" ref="A19:F33" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6B08AFF7-E6AC-487E-A862-54025ABD7D5C}" name="Tableau24" displayName="Tableau24" ref="A19:F33" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24">
   <autoFilter ref="A19:F33" xr:uid="{6B08AFF7-E6AC-487E-A862-54025ABD7D5C}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{57D8D285-6390-4ADD-8C08-C6E8212288A7}" name="Astres" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{9AA0953F-EB7A-4A32-8A2C-59A3B7D54DD6}" name="Masse" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{42C928A3-CDC0-401D-BBEB-DBDE9C296C9E}" name="Diamètre" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{F3774F47-11B7-41CC-BD67-B0851461EE8E}" name="Aplatissement" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{B4AE3617-38DD-4C16-A173-5946879F54C9}" name="Distance soleil" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{C1001996-59B6-404E-967B-839EFC3F25BB}" name="vitesse rotation équateur (km/h)" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{57D8D285-6390-4ADD-8C08-C6E8212288A7}" name="Astres" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{9AA0953F-EB7A-4A32-8A2C-59A3B7D54DD6}" name="Masse" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{42C928A3-CDC0-401D-BBEB-DBDE9C296C9E}" name="Diamètre" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{F3774F47-11B7-41CC-BD67-B0851461EE8E}" name="Aplatissement" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{B4AE3617-38DD-4C16-A173-5946879F54C9}" name="Distance soleil" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{C1001996-59B6-404E-967B-839EFC3F25BB}" name="vitesse rotation équateur (km/h)" dataDxfId="18"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CE3AC303-40F0-41E2-BA80-E1255A59C86D}" name="Tableau242" displayName="Tableau242" ref="A1:I15" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14">
+  <autoFilter ref="A1:I15" xr:uid="{CE3AC303-40F0-41E2-BA80-E1255A59C86D}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{EDE95679-AC5E-459B-B3E8-463BBC0A2BCF}" name="Astres" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{1543D1AE-2916-4C13-B130-4C9C188F65FA}" name="position x" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{BDE35151-E2B7-4D06-8610-409F0E9CE7A8}" name="position y" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{66091E47-CC13-44CA-922F-02228188114E}" name="position z" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{A0A9109F-3A5E-4113-B0C4-45A17BDE5075}" name="orbit speed = (x,y,z)" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{BEAF4F8A-6F7B-4128-8128-A05793BBD938}" name="rotation = (x,y,z)" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{8F5F32B2-D8F6-44B9-956D-C5403B260C0B}" name="OrbitRadius" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{90418A25-9A76-4ED3-861C-BA83D4A59328}" name="rotation speed = [0,0,0]" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{D0B2E9DF-29DF-408C-8213-3AD64854BC13}" name="scale" dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DBA17D35-D83C-4574-B599-94DDAA5311B4}" name="Tableau5" displayName="Tableau5" ref="J1:J15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4">
+  <autoFilter ref="J1:J15" xr:uid="{DBA17D35-D83C-4574-B599-94DDAA5311B4}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{0D6A5A56-B594-4949-9940-B1EBF208DECA}" name="texture" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1019,8 +1469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1572,4 +2022,378 @@
     <tablePart r:id="rId22"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD632101-F391-4EA6-87B1-6F8AAB6666B5}">
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="26.85546875" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="10">
+        <v>0</v>
+      </c>
+      <c r="C2" s="10">
+        <v>0</v>
+      </c>
+      <c r="D2" s="10">
+        <v>0</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="9"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="8">
+        <v>50</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="10">
+        <v>60</v>
+      </c>
+      <c r="C3" s="10">
+        <v>0</v>
+      </c>
+      <c r="D3" s="10">
+        <v>0</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="11">
+        <v>0.35034999999999999</v>
+      </c>
+      <c r="J3" s="21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="10">
+        <v>70</v>
+      </c>
+      <c r="C4" s="10">
+        <v>0</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="11">
+        <v>0.8609</v>
+      </c>
+      <c r="J4" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="10">
+        <v>80</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="10">
+        <v>80</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="10">
+        <v>0.91090000000000004</v>
+      </c>
+      <c r="J5" s="21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="10">
+        <v>90</v>
+      </c>
+      <c r="C6" s="10">
+        <v>0</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="10"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="10">
+        <v>0.48759999999999998</v>
+      </c>
+      <c r="J6" s="21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="10">
+        <v>100</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="10"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="11">
+        <v>10.2667</v>
+      </c>
+      <c r="J7" s="21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="10">
+        <v>110</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="13"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="11">
+        <v>3.5562</v>
+      </c>
+      <c r="J8" s="21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="10">
+        <v>120</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" s="21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="10">
+        <v>130</v>
+      </c>
+      <c r="C10" s="10">
+        <v>0</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="22"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="23"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="22"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="22"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="22"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="F1" r:id="rId1" display="Aplatissement" xr:uid="{58322574-E505-4A2A-8410-8BE55FBC032F}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{2B0244D5-DEF6-48A8-A99D-31A7C2184C16}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{7E2816E4-1104-421A-8534-3DB0219C7FDA}"/>
+    <hyperlink ref="A4" r:id="rId4" xr:uid="{2AF043CE-D38C-4F33-837E-C8E4147E76DD}"/>
+    <hyperlink ref="A5" r:id="rId5" xr:uid="{0A6DADD8-2F9A-4596-A7A5-EA8B54B5C746}"/>
+    <hyperlink ref="A6" r:id="rId6" xr:uid="{92F17C96-E297-44BF-AB0C-728C6B4BC239}"/>
+    <hyperlink ref="A7" r:id="rId7" xr:uid="{AF9C19CE-A559-425D-BB0B-4CA45F4408BF}"/>
+    <hyperlink ref="A8" r:id="rId8" xr:uid="{3A3161C4-F3B7-4A0C-91DC-473768F62399}"/>
+    <hyperlink ref="A9" r:id="rId9" xr:uid="{18B4E098-5C21-4E09-A5B1-0F3248FDE337}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
import des donnees excel dans le code et astres dans la base de donnees
</commit_message>
<xml_diff>
--- a/Masses astres.xlsx
+++ b/Masses astres.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bc217c0b68332ccc/Bureau/python/Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="180" documentId="13_ncr:1_{1EFD99F7-708A-4457-A218-EB357170E642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{908C2DD4-487A-4886-99FE-F815200055F0}"/>
+  <xr:revisionPtr revIDLastSave="464" documentId="13_ncr:1_{1EFD99F7-708A-4457-A218-EB357170E642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{553EEAC0-57A0-4B83-9E0F-800BD92AD403}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2520" yWindow="2370" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="61">
   <si>
     <t>Astres</t>
   </si>
@@ -90,9 +90,6 @@
     <t>vitesse rotation équateur (rad/ds)</t>
   </si>
   <si>
-    <t>paramètre orienter planète</t>
-  </si>
-  <si>
     <t>Lune</t>
   </si>
   <si>
@@ -105,48 +102,12 @@
     <t>rotation = (x,y,z)</t>
   </si>
   <si>
-    <t>orbit speed = (x,y,z)</t>
-  </si>
-  <si>
     <t>OrbitRadius</t>
   </si>
   <si>
-    <t>rotation speed = [0,0,0]</t>
-  </si>
-  <si>
     <t>texture</t>
   </si>
   <si>
-    <t>'assets/8k_sun'</t>
-  </si>
-  <si>
-    <t>'assets/mercury'</t>
-  </si>
-  <si>
-    <t>'assets/venus1'</t>
-  </si>
-  <si>
-    <t>'assets/mars'</t>
-  </si>
-  <si>
-    <t>'assets/jupiter'</t>
-  </si>
-  <si>
-    <t>'assets/saturn'</t>
-  </si>
-  <si>
-    <t>'assets/uranus'</t>
-  </si>
-  <si>
-    <t>'assets/neptune'</t>
-  </si>
-  <si>
-    <t>(360/365,0,0)</t>
-  </si>
-  <si>
-    <t>[0,-360/24,0]</t>
-  </si>
-  <si>
     <t>scale</t>
   </si>
   <si>
@@ -156,33 +117,6 @@
     <t>3.5562</t>
   </si>
   <si>
-    <t xml:space="preserve"> (23.45,0,0)</t>
-  </si>
-  <si>
-    <t>(0.03,0,0)</t>
-  </si>
-  <si>
-    <t>(7.23,0,0)</t>
-  </si>
-  <si>
-    <t>(177.36,0,0)</t>
-  </si>
-  <si>
-    <t>(25,0,0)</t>
-  </si>
-  <si>
-    <t>(1.304,0,0)</t>
-  </si>
-  <si>
-    <t>(27,0,0)</t>
-  </si>
-  <si>
-    <t>(98.32,0,0)</t>
-  </si>
-  <si>
-    <t>(28.32,0,0)</t>
-  </si>
-  <si>
     <t>assets/earth</t>
   </si>
   <si>
@@ -193,6 +127,99 @@
   </si>
   <si>
     <t>position z</t>
+  </si>
+  <si>
+    <t>Orbit speed y</t>
+  </si>
+  <si>
+    <t>Orbit speed z</t>
+  </si>
+  <si>
+    <t>rotation y</t>
+  </si>
+  <si>
+    <t>rotation z</t>
+  </si>
+  <si>
+    <t>rotation speed z</t>
+  </si>
+  <si>
+    <t>rotation speed x</t>
+  </si>
+  <si>
+    <t>orbit speed x (m/s)</t>
+  </si>
+  <si>
+    <t>assets/venus1</t>
+  </si>
+  <si>
+    <t>assets/mercury</t>
+  </si>
+  <si>
+    <t>Temps de rotation sur elle-même</t>
+  </si>
+  <si>
+    <t>Une journée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rotation speed y </t>
+  </si>
+  <si>
+    <t>assets/8k_sun</t>
+  </si>
+  <si>
+    <t>assets/mars</t>
+  </si>
+  <si>
+    <t>assets/jupiter</t>
+  </si>
+  <si>
+    <t>assets/saturn</t>
+  </si>
+  <si>
+    <t>assets/uranus</t>
+  </si>
+  <si>
+    <t>assets/neptune</t>
+  </si>
+  <si>
+    <t>47 051</t>
+  </si>
+  <si>
+    <t>34 821</t>
+  </si>
+  <si>
+    <t>9 320</t>
+  </si>
+  <si>
+    <t>9 660</t>
+  </si>
+  <si>
+    <t>Europa</t>
+  </si>
+  <si>
+    <t>Io</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calisto </t>
+  </si>
+  <si>
+    <t>Ganymède</t>
+  </si>
+  <si>
+    <t>Iapetus</t>
+  </si>
+  <si>
+    <t>Dione</t>
+  </si>
+  <si>
+    <t>Rhea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Triton </t>
+  </si>
+  <si>
+    <t>Pluto</t>
   </si>
 </sst>
 </file>
@@ -268,7 +295,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -278,6 +305,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF9F9F9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -401,7 +434,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -466,10 +499,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -478,70 +529,7 @@
     <cellStyle name="Milliers" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="47">
     <dxf>
       <font>
         <b val="0"/>
@@ -636,11 +624,88 @@
         <shadow val="0"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
+        <color auto="1"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -653,7 +718,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
@@ -662,6 +726,42 @@
         <right style="medium">
           <color indexed="64"/>
         </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -675,14 +775,43 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
         <right style="medium">
           <color indexed="64"/>
         </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -698,6 +827,75 @@
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -711,11 +909,21 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
         <right style="medium">
           <color indexed="64"/>
         </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -732,16 +940,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
+      <border>
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
@@ -761,13 +960,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -778,7 +970,16 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -791,7 +992,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
@@ -813,15 +1013,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-      </border>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -834,8 +1027,13 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -848,13 +1046,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-      </border>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -867,8 +1060,23 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -884,16 +1092,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
+      <border>
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
@@ -911,13 +1110,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1137,68 +1329,79 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{524A4480-6DAB-4CB9-8F9A-6D7582E76A58}" name="Tableau2" displayName="Tableau2" ref="A1:H15" totalsRowShown="0" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36">
-  <autoFilter ref="A1:H15" xr:uid="{524A4480-6DAB-4CB9-8F9A-6D7582E76A58}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{A3C56C48-4D56-4E78-8EAC-8A8834CCB7B6}" name="Astres" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{0ACD23B6-9D0A-41BC-9D2A-22A123127B9A}" name="Masse" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{524A4480-6DAB-4CB9-8F9A-6D7582E76A58}" name="Tableau2" displayName="Tableau2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43">
+  <autoFilter ref="A1:I15" xr:uid="{524A4480-6DAB-4CB9-8F9A-6D7582E76A58}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{A3C56C48-4D56-4E78-8EAC-8A8834CCB7B6}" name="Astres" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{0ACD23B6-9D0A-41BC-9D2A-22A123127B9A}" name="Masse" dataDxfId="41">
       <calculatedColumnFormula>1.988*10^30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{5449565D-8FF5-4D07-BC9E-A81B7DCC7C09}" name="Diamètre" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{2859AEC0-DB80-4F8A-8611-2D1CB99408B1}" name="Aplatissement" dataDxfId="32">
+    <tableColumn id="3" xr3:uid="{5449565D-8FF5-4D07-BC9E-A81B7DCC7C09}" name="Diamètre" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{2859AEC0-DB80-4F8A-8611-2D1CB99408B1}" name="Aplatissement" dataDxfId="39">
       <calculatedColumnFormula>9*10^-6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{FEFB98A5-F681-4A28-8656-83E81E4A53E3}" name="Angle de rotation (deg)" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{F49A900E-B0EE-48B7-858F-35EC2942B732}" name="vitesse rotation équateur (km/h)" dataDxfId="30">
+    <tableColumn id="6" xr3:uid="{FEFB98A5-F681-4A28-8656-83E81E4A53E3}" name="Angle de rotation (deg)" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{F49A900E-B0EE-48B7-858F-35EC2942B732}" name="vitesse rotation équateur (km/h)" dataDxfId="37">
       <calculatedColumnFormula>24*24*60*60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{7B87A2BE-ADED-4EC7-90F4-82312C153D69}" name="vitesse rotation équateur (rad/ds)" dataDxfId="29">
+    <tableColumn id="7" xr3:uid="{7B87A2BE-ADED-4EC7-90F4-82312C153D69}" name="vitesse rotation équateur (rad/ds)" dataDxfId="36">
       <calculatedColumnFormula>DEGREES((F2*1000/3600)/(C2*1000/2))/10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{2C9717ED-55F0-43A9-8BF0-C1A01A73941C}" name="paramètre orienter planète" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{2C9717ED-55F0-43A9-8BF0-C1A01A73941C}" name="Temps de rotation sur elle-même" dataDxfId="35"/>
+    <tableColumn id="9" xr3:uid="{737794A4-6A5A-4487-A0A6-9B8840488ABA}" name="Une journée" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6B08AFF7-E6AC-487E-A862-54025ABD7D5C}" name="Tableau24" displayName="Tableau24" ref="A19:F33" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6B08AFF7-E6AC-487E-A862-54025ABD7D5C}" name="Tableau24" displayName="Tableau24" ref="A19:F33" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30">
   <autoFilter ref="A19:F33" xr:uid="{6B08AFF7-E6AC-487E-A862-54025ABD7D5C}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{57D8D285-6390-4ADD-8C08-C6E8212288A7}" name="Astres" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{9AA0953F-EB7A-4A32-8A2C-59A3B7D54DD6}" name="Masse" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{42C928A3-CDC0-401D-BBEB-DBDE9C296C9E}" name="Diamètre" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{F3774F47-11B7-41CC-BD67-B0851461EE8E}" name="Aplatissement" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{B4AE3617-38DD-4C16-A173-5946879F54C9}" name="Distance soleil" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{C1001996-59B6-404E-967B-839EFC3F25BB}" name="vitesse rotation équateur (km/h)" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{57D8D285-6390-4ADD-8C08-C6E8212288A7}" name="Astres" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{9AA0953F-EB7A-4A32-8A2C-59A3B7D54DD6}" name="Masse" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{42C928A3-CDC0-401D-BBEB-DBDE9C296C9E}" name="Diamètre" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{F3774F47-11B7-41CC-BD67-B0851461EE8E}" name="Aplatissement" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{B4AE3617-38DD-4C16-A173-5946879F54C9}" name="Distance soleil" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{C1001996-59B6-404E-967B-839EFC3F25BB}" name="vitesse rotation équateur (km/h)" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CE3AC303-40F0-41E2-BA80-E1255A59C86D}" name="Tableau242" displayName="Tableau242" ref="A1:I15" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14">
-  <autoFilter ref="A1:I15" xr:uid="{CE3AC303-40F0-41E2-BA80-E1255A59C86D}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{EDE95679-AC5E-459B-B3E8-463BBC0A2BCF}" name="Astres" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{1543D1AE-2916-4C13-B130-4C9C188F65FA}" name="position x" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{BDE35151-E2B7-4D06-8610-409F0E9CE7A8}" name="position y" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{66091E47-CC13-44CA-922F-02228188114E}" name="position z" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{A0A9109F-3A5E-4113-B0C4-45A17BDE5075}" name="orbit speed = (x,y,z)" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{BEAF4F8A-6F7B-4128-8128-A05793BBD938}" name="rotation = (x,y,z)" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{8F5F32B2-D8F6-44B9-956D-C5403B260C0B}" name="OrbitRadius" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{90418A25-9A76-4ED3-861C-BA83D4A59328}" name="rotation speed = [0,0,0]" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{D0B2E9DF-29DF-408C-8213-3AD64854BC13}" name="scale" dataDxfId="8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CE3AC303-40F0-41E2-BA80-E1255A59C86D}" name="Tableau242" displayName="Tableau242" ref="A1:O21" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20">
+  <autoFilter ref="A1:O21" xr:uid="{CE3AC303-40F0-41E2-BA80-E1255A59C86D}"/>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{EDE95679-AC5E-459B-B3E8-463BBC0A2BCF}" name="Astres" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{1543D1AE-2916-4C13-B130-4C9C188F65FA}" name="position x" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{BDE35151-E2B7-4D06-8610-409F0E9CE7A8}" name="position y" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{66091E47-CC13-44CA-922F-02228188114E}" name="position z" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{A0A9109F-3A5E-4113-B0C4-45A17BDE5075}" name="orbit speed x (m/s)" dataDxfId="15">
+      <calculatedColumnFormula>360/365</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{1FB021ED-D2AE-4B20-9894-A1A7B535AF42}" name="Orbit speed y" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{6447372A-4624-4464-9007-45A417812819}" name="Orbit speed z" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{BEAF4F8A-6F7B-4128-8128-A05793BBD938}" name="rotation = (x,y,z)" dataDxfId="12"/>
+    <tableColumn id="13" xr3:uid="{B028B5E1-AA94-4521-955D-E61AE895B0ED}" name="rotation y" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{43855469-E423-4784-A5C9-DD6167279A62}" name="rotation z" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{8F5F32B2-D8F6-44B9-956D-C5403B260C0B}" name="OrbitRadius" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{90418A25-9A76-4ED3-861C-BA83D4A59328}" name="rotation speed x" dataDxfId="8"/>
+    <tableColumn id="15" xr3:uid="{D7830255-2F24-444E-9022-19DC045D5D90}" name="rotation speed y " dataDxfId="7">
+      <calculatedColumnFormula>-360/24</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="14" xr3:uid="{A8BA6684-B306-497B-A744-8A1D3880FB82}" name="rotation speed z" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{D0B2E9DF-29DF-408C-8213-3AD64854BC13}" name="scale" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DBA17D35-D83C-4574-B599-94DDAA5311B4}" name="Tableau5" displayName="Tableau5" ref="J1:J15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4">
-  <autoFilter ref="J1:J15" xr:uid="{DBA17D35-D83C-4574-B599-94DDAA5311B4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DBA17D35-D83C-4574-B599-94DDAA5311B4}" name="Tableau5" displayName="Tableau5" ref="P1:P15" totalsRowShown="0" headerRowDxfId="4" dataDxfId="2" headerRowBorderDxfId="3" tableBorderDxfId="1">
+  <autoFilter ref="P1:P15" xr:uid="{DBA17D35-D83C-4574-B599-94DDAA5311B4}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{0D6A5A56-B594-4949-9940-B1EBF208DECA}" name="texture" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{0D6A5A56-B594-4949-9940-B1EBF208DECA}" name="texture" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1467,10 +1670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1482,9 +1685,10 @@
     <col min="6" max="6" width="35.85546875" customWidth="1"/>
     <col min="7" max="7" width="27.140625" customWidth="1"/>
     <col min="8" max="8" width="29" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="58.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="58.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1498,7 +1702,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>6</v>
@@ -1507,10 +1711,13 @@
         <v>16</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>3</v>
       </c>
@@ -1526,7 +1733,7 @@
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="10">
         <f xml:space="preserve">  Tableau2[[#This Row],[Diamètre]]*2*PI()/(24.47*24)</f>
@@ -1537,8 +1744,9 @@
         <v>3.4055305816646229E-5</v>
       </c>
       <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>4</v>
       </c>
@@ -1564,8 +1772,9 @@
         <v>7.1054459161246225E-3</v>
       </c>
       <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>7</v>
       </c>
@@ -1591,8 +1800,9 @@
         <v>1.7146803082705271E-6</v>
       </c>
       <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>8</v>
       </c>
@@ -1619,8 +1829,9 @@
         <v>4.1780743677208288E-4</v>
       </c>
       <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>9</v>
       </c>
@@ -1646,8 +1857,9 @@
         <v>4.0679178623016831E-4</v>
       </c>
       <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>10</v>
       </c>
@@ -1673,8 +1885,9 @@
         <v>1.0474457600034644E-3</v>
       </c>
       <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>12</v>
       </c>
@@ -1700,8 +1913,9 @@
         <v>2.237899480456666E-3</v>
       </c>
       <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>13</v>
       </c>
@@ -1727,8 +1941,9 @@
         <v>5.8035293619330356E-4</v>
       </c>
       <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>14</v>
       </c>
@@ -1754,8 +1969,9 @@
         <v>6.2083538615236185E-4</v>
       </c>
       <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="5"/>
       <c r="C11" s="4"/>
@@ -1764,10 +1980,11 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="4"/>
@@ -1776,8 +1993,9 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="5"/>
       <c r="C13" s="4"/>
@@ -1786,8 +2004,9 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="5"/>
       <c r="C14" s="4"/>
@@ -1796,8 +2015,9 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="5"/>
       <c r="C15" s="7"/>
@@ -1806,6 +2026,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="4"/>
       <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
@@ -2026,10 +2247,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD632101-F391-4EA6-87B1-6F8AAB6666B5}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="101" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2037,47 +2258,65 @@
     <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" customWidth="1"/>
-    <col min="9" max="9" width="26.85546875" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" customWidth="1"/>
+    <col min="5" max="7" width="21.7109375" customWidth="1"/>
+    <col min="8" max="10" width="19.85546875" customWidth="1"/>
+    <col min="11" max="11" width="23.85546875" customWidth="1"/>
+    <col min="12" max="14" width="20.7109375" customWidth="1"/>
+    <col min="15" max="15" width="26.85546875" customWidth="1"/>
+    <col min="16" max="16" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>3</v>
       </c>
@@ -2090,20 +2329,44 @@
       <c r="D2" s="10">
         <v>0</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="8">
+      <c r="E2" s="9">
+        <v>1</v>
+      </c>
+      <c r="F2" s="10">
+        <v>0</v>
+      </c>
+      <c r="G2" s="10">
+        <v>0</v>
+      </c>
+      <c r="H2" s="8">
+        <v>7.23</v>
+      </c>
+      <c r="I2" s="10">
+        <v>0</v>
+      </c>
+      <c r="J2" s="10">
+        <v>0</v>
+      </c>
+      <c r="K2" s="9">
+        <v>0</v>
+      </c>
+      <c r="L2" s="10">
+        <v>0</v>
+      </c>
+      <c r="M2" s="10">
+        <v>1.9970000000000001</v>
+      </c>
+      <c r="N2" s="10">
+        <v>0</v>
+      </c>
+      <c r="O2" s="10">
         <v>50</v>
       </c>
-      <c r="J2" s="21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="P2" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>4</v>
       </c>
@@ -2116,20 +2379,44 @@
       <c r="D3" s="10">
         <v>0</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="11">
+      <c r="E3" s="10">
+        <v>1</v>
+      </c>
+      <c r="F3" s="10">
+        <v>0</v>
+      </c>
+      <c r="G3" s="10">
+        <v>0</v>
+      </c>
+      <c r="H3" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="I3" s="10">
+        <v>0</v>
+      </c>
+      <c r="J3" s="10">
+        <v>0</v>
+      </c>
+      <c r="K3" s="10">
+        <v>60</v>
+      </c>
+      <c r="L3" s="10">
+        <v>0</v>
+      </c>
+      <c r="M3" s="10">
+        <v>10.891999999999999</v>
+      </c>
+      <c r="N3" s="10">
+        <v>0</v>
+      </c>
+      <c r="O3" s="10">
         <v>0.35034999999999999</v>
       </c>
-      <c r="J3" s="21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="P3" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>7</v>
       </c>
@@ -2142,20 +2429,44 @@
       <c r="D4" s="10">
         <v>0</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="11">
+      <c r="E4" s="10">
+        <v>1</v>
+      </c>
+      <c r="F4" s="10">
+        <v>0</v>
+      </c>
+      <c r="G4" s="10">
+        <v>0</v>
+      </c>
+      <c r="H4" s="11">
+        <v>177.36</v>
+      </c>
+      <c r="I4" s="10">
+        <v>0</v>
+      </c>
+      <c r="J4" s="10">
+        <v>0</v>
+      </c>
+      <c r="K4" s="10">
+        <v>70</v>
+      </c>
+      <c r="L4" s="10">
+        <v>0</v>
+      </c>
+      <c r="M4" s="10">
+        <v>6.52</v>
+      </c>
+      <c r="N4" s="10">
+        <v>0</v>
+      </c>
+      <c r="O4" s="10">
         <v>0.8609</v>
       </c>
-      <c r="J4" s="21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="P4" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>8</v>
       </c>
@@ -2168,26 +2479,44 @@
       <c r="D5" s="10">
         <v>0</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>39</v>
+      <c r="E5" s="10">
+        <v>1</v>
+      </c>
+      <c r="F5" s="10">
+        <v>0</v>
       </c>
       <c r="G5" s="10">
+        <v>0</v>
+      </c>
+      <c r="H5" s="10">
+        <v>23.45</v>
+      </c>
+      <c r="I5" s="10">
+        <v>0</v>
+      </c>
+      <c r="J5" s="10">
+        <v>0</v>
+      </c>
+      <c r="K5" s="10">
         <v>80</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="10">
+      <c r="L5" s="10">
+        <v>0</v>
+      </c>
+      <c r="M5" s="10">
+        <v>1700</v>
+      </c>
+      <c r="N5" s="10">
+        <v>0</v>
+      </c>
+      <c r="O5" s="10">
         <v>0.91090000000000004</v>
       </c>
-      <c r="J5" s="21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="P5" s="21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>9</v>
       </c>
@@ -2200,20 +2529,44 @@
       <c r="D6" s="10">
         <v>0</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10" t="s">
+      <c r="E6" s="6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0</v>
+      </c>
+      <c r="G6" s="10">
+        <v>0</v>
+      </c>
+      <c r="H6" s="10">
+        <v>25</v>
+      </c>
+      <c r="I6" s="10">
+        <v>0</v>
+      </c>
+      <c r="J6" s="10">
+        <v>0</v>
+      </c>
+      <c r="K6" s="10">
+        <v>90</v>
+      </c>
+      <c r="L6" s="10">
+        <v>0</v>
+      </c>
+      <c r="M6" s="10">
+        <v>868.22</v>
+      </c>
+      <c r="N6" s="10">
+        <v>0</v>
+      </c>
+      <c r="O6" s="10">
+        <v>0.48759999999999998</v>
+      </c>
+      <c r="P6" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="10">
-        <v>0.48759999999999998</v>
-      </c>
-      <c r="J6" s="21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>10</v>
       </c>
@@ -2226,20 +2579,44 @@
       <c r="D7" s="10">
         <v>0</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11" t="s">
+      <c r="E7" s="10">
+        <v>1</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0</v>
+      </c>
+      <c r="G7" s="10">
+        <v>0</v>
+      </c>
+      <c r="H7" s="11">
+        <v>1.3049999999999999</v>
+      </c>
+      <c r="I7" s="10">
+        <v>0</v>
+      </c>
+      <c r="J7" s="10">
+        <v>0</v>
+      </c>
+      <c r="K7" s="10">
+        <v>100</v>
+      </c>
+      <c r="L7" s="10">
+        <v>0</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="N7" s="10">
+        <v>0</v>
+      </c>
+      <c r="O7" s="10">
+        <v>10.2667</v>
+      </c>
+      <c r="P7" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="11">
-        <v>10.2667</v>
-      </c>
-      <c r="J7" s="21" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>12</v>
       </c>
@@ -2252,20 +2629,44 @@
       <c r="D8" s="10">
         <v>0</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="11" t="s">
+      <c r="E8" s="10">
+        <v>1</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0</v>
+      </c>
+      <c r="H8" s="11">
+        <v>27</v>
+      </c>
+      <c r="I8" s="10">
+        <v>0</v>
+      </c>
+      <c r="J8" s="10">
+        <v>0</v>
+      </c>
+      <c r="K8" s="13">
+        <v>110</v>
+      </c>
+      <c r="L8" s="10">
+        <v>0</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="N8" s="10">
+        <v>0</v>
+      </c>
+      <c r="O8" s="10">
+        <v>3.5562</v>
+      </c>
+      <c r="P8" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="13"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="11">
-        <v>3.5562</v>
-      </c>
-      <c r="J8" s="21" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>13</v>
       </c>
@@ -2278,20 +2679,44 @@
       <c r="D9" s="10">
         <v>0</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="11" t="s">
+      <c r="E9" s="10">
+        <v>1</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0</v>
+      </c>
+      <c r="G9" s="10">
+        <v>0</v>
+      </c>
+      <c r="H9" s="11">
+        <v>98.32</v>
+      </c>
+      <c r="I9" s="10">
+        <v>0</v>
+      </c>
+      <c r="J9" s="10">
+        <v>0</v>
+      </c>
+      <c r="K9" s="10">
+        <v>120</v>
+      </c>
+      <c r="L9" s="10">
+        <v>0</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="N9" s="10">
+        <v>0</v>
+      </c>
+      <c r="O9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="P9" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="J9" s="21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>14</v>
       </c>
@@ -2304,83 +2729,411 @@
       <c r="D10" s="10">
         <v>0</v>
       </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="4" t="s">
+      <c r="E10" s="10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="10">
+        <v>0</v>
+      </c>
+      <c r="G10" s="10">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4">
+        <v>28.32</v>
+      </c>
+      <c r="I10" s="10">
+        <v>0</v>
+      </c>
+      <c r="J10" s="10">
+        <v>0</v>
+      </c>
+      <c r="K10" s="10">
+        <v>130</v>
+      </c>
+      <c r="L10" s="10">
+        <v>0</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="N10" s="10">
+        <v>0</v>
+      </c>
+      <c r="O10" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="P10" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="J10" s="21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="22"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="26"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="27">
+        <v>0</v>
+      </c>
+      <c r="M11" s="27"/>
+      <c r="N11" s="27"/>
+      <c r="O11" s="27"/>
+      <c r="P11" s="29"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="23"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
+      <c r="E12" s="4">
+        <v>1</v>
+      </c>
+      <c r="F12" s="10">
+        <v>0</v>
+      </c>
+      <c r="G12" s="10">
+        <v>0</v>
+      </c>
+      <c r="H12" s="4">
+        <v>5.14</v>
+      </c>
+      <c r="I12" s="10">
+        <v>0</v>
+      </c>
+      <c r="J12" s="10">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4"/>
+      <c r="L12" s="10">
+        <v>0</v>
+      </c>
+      <c r="M12" s="10">
+        <v>16.7</v>
+      </c>
+      <c r="N12" s="10">
+        <v>0</v>
+      </c>
+      <c r="O12" s="10"/>
+      <c r="P12" s="22"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="22"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
+      <c r="E13" s="4">
+        <v>1</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0</v>
+      </c>
+      <c r="G13" s="10">
+        <v>0</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="10">
+        <v>0</v>
+      </c>
+      <c r="J13" s="10">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4"/>
+      <c r="L13" s="10">
+        <v>0</v>
+      </c>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10">
+        <v>0</v>
+      </c>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="22"/>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
-      <c r="B15" s="10"/>
+      <c r="E14" s="10">
+        <v>1</v>
+      </c>
+      <c r="F14" s="10">
+        <v>0</v>
+      </c>
+      <c r="G14" s="10">
+        <v>0</v>
+      </c>
+      <c r="H14" s="5"/>
+      <c r="I14" s="10">
+        <v>0</v>
+      </c>
+      <c r="J14" s="10">
+        <v>0</v>
+      </c>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10">
+        <v>0</v>
+      </c>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10">
+        <v>0</v>
+      </c>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="4"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="22"/>
+      <c r="E15" s="10">
+        <v>1</v>
+      </c>
+      <c r="F15" s="10">
+        <v>0</v>
+      </c>
+      <c r="G15" s="10">
+        <v>0</v>
+      </c>
+      <c r="H15" s="5"/>
+      <c r="I15" s="10">
+        <v>0</v>
+      </c>
+      <c r="J15" s="10">
+        <v>0</v>
+      </c>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10">
+        <v>0</v>
+      </c>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10">
+        <v>0</v>
+      </c>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10">
+        <v>1</v>
+      </c>
+      <c r="F16" s="10">
+        <v>0</v>
+      </c>
+      <c r="G16" s="10">
+        <v>0</v>
+      </c>
+      <c r="H16" s="25"/>
+      <c r="I16" s="10">
+        <v>0</v>
+      </c>
+      <c r="J16" s="10">
+        <v>0</v>
+      </c>
+      <c r="K16" s="10"/>
+      <c r="L16" s="24">
+        <v>0</v>
+      </c>
+      <c r="M16" s="24"/>
+      <c r="N16" s="10">
+        <v>0</v>
+      </c>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10">
+        <v>1</v>
+      </c>
+      <c r="F17" s="10">
+        <v>0</v>
+      </c>
+      <c r="G17" s="10">
+        <v>0</v>
+      </c>
+      <c r="H17" s="25"/>
+      <c r="I17" s="10">
+        <v>0</v>
+      </c>
+      <c r="J17" s="10">
+        <v>0</v>
+      </c>
+      <c r="K17" s="10"/>
+      <c r="L17" s="24">
+        <v>0</v>
+      </c>
+      <c r="M17" s="24"/>
+      <c r="N17" s="10">
+        <v>0</v>
+      </c>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10">
+        <v>1</v>
+      </c>
+      <c r="F18" s="10">
+        <v>0</v>
+      </c>
+      <c r="G18" s="10">
+        <v>0</v>
+      </c>
+      <c r="H18" s="25"/>
+      <c r="I18" s="10">
+        <v>0</v>
+      </c>
+      <c r="J18" s="10">
+        <v>0</v>
+      </c>
+      <c r="K18" s="10"/>
+      <c r="L18" s="24">
+        <v>0</v>
+      </c>
+      <c r="M18" s="24"/>
+      <c r="N18" s="10">
+        <v>0</v>
+      </c>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="24"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10">
+        <v>1</v>
+      </c>
+      <c r="F19" s="10">
+        <v>0</v>
+      </c>
+      <c r="G19" s="10">
+        <v>0</v>
+      </c>
+      <c r="H19" s="25"/>
+      <c r="I19" s="10">
+        <v>0</v>
+      </c>
+      <c r="J19" s="10">
+        <v>0</v>
+      </c>
+      <c r="K19" s="10"/>
+      <c r="L19" s="24">
+        <v>0</v>
+      </c>
+      <c r="M19" s="24"/>
+      <c r="N19" s="10">
+        <v>0</v>
+      </c>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="24"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10">
+        <v>1</v>
+      </c>
+      <c r="F20" s="10">
+        <v>0</v>
+      </c>
+      <c r="G20" s="10">
+        <v>0</v>
+      </c>
+      <c r="H20" s="25"/>
+      <c r="I20" s="10">
+        <v>0</v>
+      </c>
+      <c r="J20" s="10">
+        <v>0</v>
+      </c>
+      <c r="K20" s="10"/>
+      <c r="L20" s="24">
+        <v>0</v>
+      </c>
+      <c r="M20" s="24"/>
+      <c r="N20" s="10">
+        <v>0</v>
+      </c>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="24"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10">
+        <v>1</v>
+      </c>
+      <c r="F21" s="10">
+        <v>0</v>
+      </c>
+      <c r="G21" s="10">
+        <v>0</v>
+      </c>
+      <c r="H21" s="25"/>
+      <c r="I21" s="10">
+        <v>0</v>
+      </c>
+      <c r="J21" s="10">
+        <v>0</v>
+      </c>
+      <c r="K21" s="10"/>
+      <c r="L21" s="24">
+        <v>0</v>
+      </c>
+      <c r="M21" s="24"/>
+      <c r="N21" s="10">
+        <v>0</v>
+      </c>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F1" r:id="rId1" display="Aplatissement" xr:uid="{58322574-E505-4A2A-8410-8BE55FBC032F}"/>
+    <hyperlink ref="H1" r:id="rId1" display="Aplatissement" xr:uid="{58322574-E505-4A2A-8410-8BE55FBC032F}"/>
     <hyperlink ref="A2" r:id="rId2" xr:uid="{2B0244D5-DEF6-48A8-A99D-31A7C2184C16}"/>
     <hyperlink ref="A3" r:id="rId3" xr:uid="{7E2816E4-1104-421A-8534-3DB0219C7FDA}"/>
     <hyperlink ref="A4" r:id="rId4" xr:uid="{2AF043CE-D38C-4F33-837E-C8E4147E76DD}"/>

</xml_diff>

<commit_message>
loop for planets and sun creation
</commit_message>
<xml_diff>
--- a/Masses astres.xlsx
+++ b/Masses astres.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mael2\Desktop\Git\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8262F406-2AEC-4F74-A663-977B70CECD46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8198026-338D-4AF0-91D7-0A7C60F2BC96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5784" yWindow="0" windowWidth="17256" windowHeight="9420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="72">
   <si>
     <t>Astres</t>
   </si>
@@ -169,18 +169,6 @@
   </si>
   <si>
     <t>assets/neptune</t>
-  </si>
-  <si>
-    <t>47 051</t>
-  </si>
-  <si>
-    <t>34 821</t>
-  </si>
-  <si>
-    <t>9 320</t>
-  </si>
-  <si>
-    <t>9 660</t>
   </si>
   <si>
     <t>Europa</t>
@@ -520,7 +508,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -643,6 +631,13 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
@@ -694,7 +689,7 @@
         <color auto="1"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -703,17 +698,15 @@
         </right>
         <top/>
         <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
       <font>
         <color auto="1"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -722,8 +715,6 @@
         </right>
         <top/>
         <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -740,7 +731,7 @@
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -749,8 +740,6 @@
         </right>
         <top/>
         <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1790,13 +1779,13 @@
         <v>16</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I1" s="23" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -1829,7 +1818,7 @@
         <v>0</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J2" s="4"/>
     </row>
@@ -1859,10 +1848,10 @@
         <v>7.1054459161246225E-3</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J3" s="4"/>
     </row>
@@ -1892,10 +1881,10 @@
         <v>1.7146803082705271E-6</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J4" s="4"/>
     </row>
@@ -1926,10 +1915,10 @@
         <v>4.1780743677208288E-4</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J5" s="4"/>
     </row>
@@ -1963,7 +1952,7 @@
         <v>226000000</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J6" s="4"/>
     </row>
@@ -1997,7 +1986,7 @@
         <v>778600000</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J7" s="4"/>
     </row>
@@ -2027,10 +2016,10 @@
         <v>2.237899480456666E-3</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J8" s="4"/>
     </row>
@@ -2060,10 +2049,10 @@
         <v>5.8035293619330356E-4</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J9" s="4"/>
     </row>
@@ -2093,10 +2082,10 @@
         <v>6.2083538615236185E-4</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J10" s="4"/>
     </row>
@@ -2133,21 +2122,21 @@
         <v>16.7</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I12" s="9">
         <v>384400</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="26" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B13" s="9">
         <f>4.8 * 10^22</f>
@@ -2158,7 +2147,7 @@
         <v>3121.6</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E13" s="9">
         <v>0.46899999999999997</v>
@@ -2168,7 +2157,7 @@
         <v>115.37406620524585</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H13" s="9">
         <f>270*10^6</f>
@@ -2178,12 +2167,12 @@
         <v>671000</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B14" s="9">
         <f>8.9319*10^22</f>
@@ -2194,7 +2183,7 @@
         <v>3643.2</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E14" s="9">
         <v>3.5999999999999997E-2</v>
@@ -2204,7 +2193,7 @@
         <v>269.30471424843137</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H14" s="9">
         <f>778*10^6</f>
@@ -2214,12 +2203,12 @@
         <v>442000</v>
       </c>
       <c r="J14" s="24" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="26" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B15" s="9">
         <f>1.2 * 10^17</f>
@@ -2227,12 +2216,12 @@
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="9"/>
       <c r="G15" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="5"/>
@@ -2240,7 +2229,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="27" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B16" s="9">
         <f>1.4819*10^23</f>
@@ -2248,12 +2237,12 @@
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="9"/>
       <c r="G16" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="5"/>
@@ -2261,7 +2250,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="28" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B17" s="9">
         <f>1.88*10^21</f>
@@ -2269,12 +2258,12 @@
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="9"/>
       <c r="G17" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H17" s="9"/>
       <c r="I17" s="5"/>
@@ -2282,7 +2271,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B18" s="9">
         <f>1.096 * 10^21</f>
@@ -2293,7 +2282,7 @@
         <v>1118</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E18" s="5">
         <v>2E-3</v>
@@ -2302,21 +2291,21 @@
         <v>56.73</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I18" s="24">
         <v>377400</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="28" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B19" s="11">
         <f>2.306518 * 10^21</f>
@@ -2324,12 +2313,12 @@
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="9"/>
       <c r="G19" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="5"/>
@@ -2337,7 +2326,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="27" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B20" s="9">
         <f>2.14 * 10^22</f>
@@ -2345,12 +2334,12 @@
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="9"/>
       <c r="G20" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H20" s="9"/>
       <c r="I20" s="5"/>
@@ -2358,7 +2347,7 @@
     </row>
     <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="29" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B21" s="9">
         <f>1.29*10^22</f>
@@ -2366,17 +2355,17 @@
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H21" s="9"/>
       <c r="I21" s="5"/>
       <c r="J21" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -2420,7 +2409,7 @@
         <v>6</v>
       </c>
       <c r="G25" s="23" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -2435,7 +2424,7 @@
       <c r="E26" s="8"/>
       <c r="F26" s="9"/>
       <c r="G26" s="31" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -2451,7 +2440,7 @@
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
       <c r="G27" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -2467,7 +2456,7 @@
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
       <c r="G28" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -2483,7 +2472,7 @@
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
       <c r="G29" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
@@ -2499,7 +2488,7 @@
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
       <c r="G30" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
@@ -2515,7 +2504,7 @@
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
       <c r="G31" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
@@ -2531,7 +2520,7 @@
       <c r="E32" s="11"/>
       <c r="F32" s="9"/>
       <c r="G32" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -2547,7 +2536,7 @@
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
       <c r="G33" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -2563,7 +2552,7 @@
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
       <c r="G34" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -2591,7 +2580,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="26" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
@@ -2602,7 +2591,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="25" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
@@ -2613,7 +2602,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="26" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
@@ -2624,7 +2613,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="27" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
@@ -2635,7 +2624,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="28" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B41" s="11"/>
       <c r="C41" s="9"/>
@@ -2646,7 +2635,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="27" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B42" s="9"/>
       <c r="C42" s="11">
@@ -2660,7 +2649,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="28" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
@@ -2671,7 +2660,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="27" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
@@ -2682,7 +2671,7 @@
     </row>
     <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="29" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
@@ -2729,8 +2718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD632101-F391-4EA6-87B1-6F8AAB6666B5}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2741,7 +2730,9 @@
     <col min="5" max="7" width="21.6640625" customWidth="1"/>
     <col min="8" max="10" width="19.88671875" customWidth="1"/>
     <col min="11" max="11" width="23.88671875" customWidth="1"/>
-    <col min="12" max="14" width="20.6640625" customWidth="1"/>
+    <col min="12" max="12" width="20.6640625" customWidth="1"/>
+    <col min="13" max="13" width="20.6640625" style="44" customWidth="1"/>
+    <col min="14" max="14" width="20.6640625" customWidth="1"/>
     <col min="15" max="15" width="26.88671875" customWidth="1"/>
     <col min="16" max="16" width="17.33203125" customWidth="1"/>
   </cols>
@@ -2769,7 +2760,7 @@
         <v>29</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="I1" s="16" t="s">
         <v>30</v>
@@ -2783,7 +2774,7 @@
       <c r="L1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="43" t="s">
         <v>37</v>
       </c>
       <c r="N1" s="3" t="s">
@@ -2793,7 +2784,7 @@
         <v>21</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
@@ -2834,7 +2825,7 @@
       <c r="L2" s="9">
         <v>0</v>
       </c>
-      <c r="M2" s="9">
+      <c r="M2" s="38">
         <v>3600</v>
       </c>
       <c r="N2" s="9">
@@ -2885,7 +2876,7 @@
       <c r="L3" s="9">
         <v>0</v>
       </c>
-      <c r="M3" s="9">
+      <c r="M3" s="38">
         <v>10.891999999999999</v>
       </c>
       <c r="N3" s="9">
@@ -2936,7 +2927,7 @@
       <c r="L4" s="9">
         <v>0</v>
       </c>
-      <c r="M4" s="9">
+      <c r="M4" s="38">
         <v>6.52</v>
       </c>
       <c r="N4" s="9">
@@ -2987,7 +2978,7 @@
       <c r="L5" s="9">
         <v>0</v>
       </c>
-      <c r="M5" s="9">
+      <c r="M5" s="38">
         <v>1674.364</v>
       </c>
       <c r="N5" s="9">
@@ -3038,7 +3029,7 @@
       <c r="L6" s="9">
         <v>0</v>
       </c>
-      <c r="M6" s="9">
+      <c r="M6" s="38">
         <v>868.22</v>
       </c>
       <c r="N6" s="9">
@@ -3089,8 +3080,8 @@
       <c r="L7" s="9">
         <v>0</v>
       </c>
-      <c r="M7" s="9" t="s">
-        <v>44</v>
+      <c r="M7" s="38">
+        <v>47051</v>
       </c>
       <c r="N7" s="9">
         <v>0</v>
@@ -3140,8 +3131,8 @@
       <c r="L8" s="9">
         <v>0</v>
       </c>
-      <c r="M8" s="9" t="s">
-        <v>45</v>
+      <c r="M8" s="38">
+        <v>34821</v>
       </c>
       <c r="N8" s="9">
         <v>0</v>
@@ -3191,8 +3182,8 @@
       <c r="L9" s="9">
         <v>0</v>
       </c>
-      <c r="M9" s="9" t="s">
-        <v>46</v>
+      <c r="M9" s="38">
+        <v>9320</v>
       </c>
       <c r="N9" s="9">
         <v>0</v>
@@ -3242,8 +3233,8 @@
       <c r="L10" s="9">
         <v>0</v>
       </c>
-      <c r="M10" s="9" t="s">
-        <v>47</v>
+      <c r="M10" s="38">
+        <v>9660</v>
       </c>
       <c r="N10" s="9">
         <v>0</v>
@@ -3273,7 +3264,7 @@
       <c r="L11" s="19">
         <v>0</v>
       </c>
-      <c r="M11" s="19"/>
+      <c r="M11" s="42"/>
       <c r="N11" s="19"/>
       <c r="O11" s="19"/>
       <c r="P11" s="21"/>
@@ -3316,7 +3307,7 @@
       <c r="L12" s="9">
         <v>0</v>
       </c>
-      <c r="M12" s="9">
+      <c r="M12" s="38">
         <v>16.7</v>
       </c>
       <c r="N12" s="9">
@@ -3326,12 +3317,12 @@
         <v>0.02</v>
       </c>
       <c r="P12" s="17" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -3359,7 +3350,7 @@
       <c r="L13" s="9">
         <v>0</v>
       </c>
-      <c r="M13" s="9"/>
+      <c r="M13" s="38"/>
       <c r="N13" s="9">
         <v>0</v>
       </c>
@@ -3368,7 +3359,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -3396,7 +3387,7 @@
       <c r="L14" s="9">
         <v>0</v>
       </c>
-      <c r="M14" s="9"/>
+      <c r="M14" s="38"/>
       <c r="N14" s="9">
         <v>0</v>
       </c>
@@ -3405,7 +3396,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="9"/>
@@ -3433,7 +3424,7 @@
       <c r="L15" s="9">
         <v>0</v>
       </c>
-      <c r="M15" s="9"/>
+      <c r="M15" s="38"/>
       <c r="N15" s="9">
         <v>0</v>
       </c>
@@ -3442,7 +3433,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="9"/>
@@ -3470,7 +3461,7 @@
       <c r="L16" s="9">
         <v>0</v>
       </c>
-      <c r="M16" s="9"/>
+      <c r="M16" s="38"/>
       <c r="N16" s="9">
         <v>0</v>
       </c>
@@ -3479,7 +3470,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="9"/>
@@ -3507,7 +3498,7 @@
       <c r="L17" s="9">
         <v>0</v>
       </c>
-      <c r="M17" s="9"/>
+      <c r="M17" s="38"/>
       <c r="N17" s="9">
         <v>0</v>
       </c>
@@ -3516,7 +3507,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B18" s="4">
         <v>110</v>
@@ -3552,7 +3543,7 @@
       <c r="L18" s="9">
         <v>0</v>
       </c>
-      <c r="M18" s="9">
+      <c r="M18" s="38">
         <v>53.73</v>
       </c>
       <c r="N18" s="9">
@@ -3562,12 +3553,12 @@
         <v>0.9</v>
       </c>
       <c r="P18" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -3595,7 +3586,7 @@
       <c r="L19" s="9">
         <v>0</v>
       </c>
-      <c r="M19" s="9"/>
+      <c r="M19" s="38"/>
       <c r="N19" s="9">
         <v>0</v>
       </c>
@@ -3604,7 +3595,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -3632,7 +3623,7 @@
       <c r="L20" s="9">
         <v>0</v>
       </c>
-      <c r="M20" s="9"/>
+      <c r="M20" s="38"/>
       <c r="N20" s="9">
         <v>0</v>
       </c>
@@ -3641,7 +3632,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -3669,7 +3660,7 @@
       <c r="L21" s="9">
         <v>0</v>
       </c>
-      <c r="M21" s="9"/>
+      <c r="M21" s="38"/>
       <c r="N21" s="9">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
file management nas loop
</commit_message>
<xml_diff>
--- a/Masses astres.xlsx
+++ b/Masses astres.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mael2\Desktop\Git\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8198026-338D-4AF0-91D7-0A7C60F2BC96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B522A1C-7A4B-4447-A0D9-EFC2CB1FEDC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -111,9 +111,6 @@
     <t>3.5562</t>
   </si>
   <si>
-    <t>assets/earth</t>
-  </si>
-  <si>
     <t>position x</t>
   </si>
   <si>
@@ -144,33 +141,9 @@
     <t>orbit speed x (m/s)</t>
   </si>
   <si>
-    <t>assets/venus1</t>
-  </si>
-  <si>
-    <t>assets/mercury</t>
-  </si>
-  <si>
     <t xml:space="preserve">rotation speed y </t>
   </si>
   <si>
-    <t>assets/8k_sun</t>
-  </si>
-  <si>
-    <t>assets/mars</t>
-  </si>
-  <si>
-    <t>assets/jupiter</t>
-  </si>
-  <si>
-    <t>assets/saturn</t>
-  </si>
-  <si>
-    <t>assets/uranus</t>
-  </si>
-  <si>
-    <t>assets/neptune</t>
-  </si>
-  <si>
     <t>Europa</t>
   </si>
   <si>
@@ -198,9 +171,6 @@
     <t>Pluto</t>
   </si>
   <si>
-    <t>assets/Moon</t>
-  </si>
-  <si>
     <t>Texture</t>
   </si>
   <si>
@@ -231,9 +201,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>assets/dione</t>
-  </si>
-  <si>
     <t>Distance planète-satellite</t>
   </si>
   <si>
@@ -253,6 +220,39 @@
   </si>
   <si>
     <t>rotation x</t>
+  </si>
+  <si>
+    <t>assets/textures/8k_sun</t>
+  </si>
+  <si>
+    <t>assets/textures/mercury</t>
+  </si>
+  <si>
+    <t>assets/textures/venus1</t>
+  </si>
+  <si>
+    <t>assets/textures/earth</t>
+  </si>
+  <si>
+    <t>assets/textures/mars</t>
+  </si>
+  <si>
+    <t>assets/textures/jupiter</t>
+  </si>
+  <si>
+    <t>assets/textures/saturn</t>
+  </si>
+  <si>
+    <t>assets/textures/uranus</t>
+  </si>
+  <si>
+    <t>assets/textures/neptune</t>
+  </si>
+  <si>
+    <t>assets/textures/Moon</t>
+  </si>
+  <si>
+    <t>assets/textures/dione</t>
   </si>
 </sst>
 </file>
@@ -508,7 +508,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -638,6 +638,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
@@ -1779,13 +1785,13 @@
         <v>16</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="I1" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -1818,7 +1824,7 @@
         <v>0</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="J2" s="4"/>
     </row>
@@ -1848,10 +1854,10 @@
         <v>7.1054459161246225E-3</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="J3" s="4"/>
     </row>
@@ -1881,10 +1887,10 @@
         <v>1.7146803082705271E-6</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="J4" s="4"/>
     </row>
@@ -1915,10 +1921,10 @@
         <v>4.1780743677208288E-4</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="J5" s="4"/>
     </row>
@@ -1952,7 +1958,7 @@
         <v>226000000</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="J6" s="4"/>
     </row>
@@ -1986,7 +1992,7 @@
         <v>778600000</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="J7" s="4"/>
     </row>
@@ -2016,10 +2022,10 @@
         <v>2.237899480456666E-3</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="J8" s="4"/>
     </row>
@@ -2049,10 +2055,10 @@
         <v>5.8035293619330356E-4</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="J9" s="4"/>
     </row>
@@ -2082,10 +2088,10 @@
         <v>6.2083538615236185E-4</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="J10" s="4"/>
     </row>
@@ -2122,21 +2128,21 @@
         <v>16.7</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="I12" s="9">
         <v>384400</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="26" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B13" s="9">
         <f>4.8 * 10^22</f>
@@ -2147,7 +2153,7 @@
         <v>3121.6</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E13" s="9">
         <v>0.46899999999999997</v>
@@ -2157,7 +2163,7 @@
         <v>115.37406620524585</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="H13" s="9">
         <f>270*10^6</f>
@@ -2167,12 +2173,12 @@
         <v>671000</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B14" s="9">
         <f>8.9319*10^22</f>
@@ -2183,7 +2189,7 @@
         <v>3643.2</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E14" s="9">
         <v>3.5999999999999997E-2</v>
@@ -2193,7 +2199,7 @@
         <v>269.30471424843137</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="H14" s="9">
         <f>778*10^6</f>
@@ -2203,12 +2209,12 @@
         <v>442000</v>
       </c>
       <c r="J14" s="24" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="26" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B15" s="9">
         <f>1.2 * 10^17</f>
@@ -2216,12 +2222,12 @@
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="9" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="9"/>
       <c r="G15" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="5"/>
@@ -2229,7 +2235,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="27" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B16" s="9">
         <f>1.4819*10^23</f>
@@ -2237,12 +2243,12 @@
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="9" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="9"/>
       <c r="G16" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="5"/>
@@ -2250,7 +2256,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="28" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B17" s="9">
         <f>1.88*10^21</f>
@@ -2258,12 +2264,12 @@
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="9" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="9"/>
       <c r="G17" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="H17" s="9"/>
       <c r="I17" s="5"/>
@@ -2271,7 +2277,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B18" s="9">
         <f>1.096 * 10^21</f>
@@ -2282,7 +2288,7 @@
         <v>1118</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E18" s="5">
         <v>2E-3</v>
@@ -2291,21 +2297,21 @@
         <v>56.73</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="I18" s="24">
         <v>377400</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="28" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B19" s="11">
         <f>2.306518 * 10^21</f>
@@ -2313,12 +2319,12 @@
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="9" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="9"/>
       <c r="G19" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="5"/>
@@ -2326,7 +2332,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="27" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B20" s="9">
         <f>2.14 * 10^22</f>
@@ -2334,12 +2340,12 @@
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="9"/>
       <c r="G20" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="H20" s="9"/>
       <c r="I20" s="5"/>
@@ -2347,7 +2353,7 @@
     </row>
     <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="29" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B21" s="9">
         <f>1.29*10^22</f>
@@ -2355,17 +2361,17 @@
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="H21" s="9"/>
       <c r="I21" s="5"/>
       <c r="J21" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -2409,7 +2415,7 @@
         <v>6</v>
       </c>
       <c r="G25" s="23" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -2424,7 +2430,7 @@
       <c r="E26" s="8"/>
       <c r="F26" s="9"/>
       <c r="G26" s="31" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -2440,7 +2446,7 @@
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
       <c r="G27" s="5" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -2456,7 +2462,7 @@
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
       <c r="G28" s="5" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -2472,7 +2478,7 @@
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
       <c r="G29" s="5" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
@@ -2488,7 +2494,7 @@
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
       <c r="G30" s="5" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
@@ -2504,7 +2510,7 @@
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
       <c r="G31" s="5" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
@@ -2520,7 +2526,7 @@
       <c r="E32" s="11"/>
       <c r="F32" s="9"/>
       <c r="G32" s="5" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -2536,7 +2542,7 @@
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
       <c r="G33" s="5" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -2552,7 +2558,7 @@
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
       <c r="G34" s="5" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -2580,7 +2586,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="26" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
@@ -2591,7 +2597,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="25" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
@@ -2602,7 +2608,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="26" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
@@ -2613,7 +2619,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="27" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
@@ -2624,7 +2630,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="28" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B41" s="11"/>
       <c r="C41" s="9"/>
@@ -2635,7 +2641,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="27" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B42" s="9"/>
       <c r="C42" s="11">
@@ -2649,7 +2655,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="28" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
@@ -2660,7 +2666,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="27" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
@@ -2671,7 +2677,7 @@
     </row>
     <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="29" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
@@ -2719,7 +2725,7 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2742,49 +2748,49 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1" s="16" t="s">
+      <c r="J1" s="16" t="s">
         <v>30</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>31</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M1" s="43" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O1" s="16" t="s">
         <v>21</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
@@ -2835,7 +2841,7 @@
         <v>100</v>
       </c>
       <c r="P2" s="17" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -2886,7 +2892,7 @@
         <v>0.35034999999999999</v>
       </c>
       <c r="P3" s="17" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -2937,7 +2943,7 @@
         <v>0.8609</v>
       </c>
       <c r="P4" s="17" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -2988,7 +2994,7 @@
         <v>0.91090000000000004</v>
       </c>
       <c r="P5" s="17" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
@@ -3039,7 +3045,7 @@
         <v>0.48759999999999998</v>
       </c>
       <c r="P6" s="17" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
@@ -3090,7 +3096,7 @@
         <v>10.2667</v>
       </c>
       <c r="P7" s="17" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
@@ -3141,7 +3147,7 @@
         <v>3.5562</v>
       </c>
       <c r="P8" s="17" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
@@ -3192,7 +3198,7 @@
         <v>22</v>
       </c>
       <c r="P9" s="17" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
@@ -3243,7 +3249,7 @@
         <v>23</v>
       </c>
       <c r="P10" s="17" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
@@ -3317,16 +3323,22 @@
         <v>0.02</v>
       </c>
       <c r="P12" s="17" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
+        <v>35</v>
+      </c>
+      <c r="B13" s="9">
+        <v>0</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0</v>
+      </c>
       <c r="E13" s="4">
         <v>1</v>
       </c>
@@ -3336,7 +3348,9 @@
       <c r="G13" s="9">
         <v>0</v>
       </c>
-      <c r="H13" s="41"/>
+      <c r="H13" s="9">
+        <v>0</v>
+      </c>
       <c r="I13" s="9">
         <v>0</v>
       </c>
@@ -3350,20 +3364,32 @@
       <c r="L13" s="9">
         <v>0</v>
       </c>
-      <c r="M13" s="38"/>
+      <c r="M13" s="9">
+        <v>0</v>
+      </c>
       <c r="N13" s="9">
         <v>0</v>
       </c>
-      <c r="O13" s="9"/>
-      <c r="P13" s="5"/>
+      <c r="O13" s="9">
+        <v>0</v>
+      </c>
+      <c r="P13" s="45">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
+        <v>36</v>
+      </c>
+      <c r="B14" s="9">
+        <v>0</v>
+      </c>
+      <c r="C14" s="9">
+        <v>0</v>
+      </c>
+      <c r="D14" s="9">
+        <v>0</v>
+      </c>
       <c r="E14" s="9">
         <v>1</v>
       </c>
@@ -3373,7 +3399,9 @@
       <c r="G14" s="9">
         <v>0</v>
       </c>
-      <c r="H14" s="41"/>
+      <c r="H14" s="9">
+        <v>0</v>
+      </c>
       <c r="I14" s="9">
         <v>0</v>
       </c>
@@ -3387,20 +3415,32 @@
       <c r="L14" s="9">
         <v>0</v>
       </c>
-      <c r="M14" s="38"/>
+      <c r="M14" s="9">
+        <v>0</v>
+      </c>
       <c r="N14" s="9">
         <v>0</v>
       </c>
-      <c r="O14" s="9"/>
-      <c r="P14" s="5"/>
+      <c r="O14" s="9">
+        <v>0</v>
+      </c>
+      <c r="P14" s="45">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
+        <v>37</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0</v>
+      </c>
+      <c r="C15" s="9">
+        <v>0</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0</v>
+      </c>
       <c r="E15" s="9">
         <v>1</v>
       </c>
@@ -3410,7 +3450,9 @@
       <c r="G15" s="9">
         <v>0</v>
       </c>
-      <c r="H15" s="41"/>
+      <c r="H15" s="9">
+        <v>0</v>
+      </c>
       <c r="I15" s="9">
         <v>0</v>
       </c>
@@ -3424,20 +3466,32 @@
       <c r="L15" s="9">
         <v>0</v>
       </c>
-      <c r="M15" s="38"/>
+      <c r="M15" s="9">
+        <v>0</v>
+      </c>
       <c r="N15" s="9">
         <v>0</v>
       </c>
-      <c r="O15" s="9"/>
-      <c r="P15" s="5"/>
+      <c r="O15" s="9">
+        <v>0</v>
+      </c>
+      <c r="P15" s="45">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
+        <v>38</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0</v>
+      </c>
+      <c r="C16" s="9">
+        <v>0</v>
+      </c>
+      <c r="D16" s="9">
+        <v>0</v>
+      </c>
       <c r="E16" s="9">
         <v>1</v>
       </c>
@@ -3447,7 +3501,9 @@
       <c r="G16" s="9">
         <v>0</v>
       </c>
-      <c r="H16" s="41"/>
+      <c r="H16" s="9">
+        <v>0</v>
+      </c>
       <c r="I16" s="9">
         <v>0</v>
       </c>
@@ -3461,20 +3517,32 @@
       <c r="L16" s="9">
         <v>0</v>
       </c>
-      <c r="M16" s="38"/>
+      <c r="M16" s="9">
+        <v>0</v>
+      </c>
       <c r="N16" s="9">
         <v>0</v>
       </c>
-      <c r="O16" s="9"/>
-      <c r="P16" s="5"/>
+      <c r="O16" s="9">
+        <v>0</v>
+      </c>
+      <c r="P16" s="45">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
+        <v>39</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0</v>
+      </c>
+      <c r="C17" s="9">
+        <v>0</v>
+      </c>
+      <c r="D17" s="9">
+        <v>0</v>
+      </c>
       <c r="E17" s="9">
         <v>1</v>
       </c>
@@ -3484,7 +3552,9 @@
       <c r="G17" s="9">
         <v>0</v>
       </c>
-      <c r="H17" s="41"/>
+      <c r="H17" s="9">
+        <v>0</v>
+      </c>
       <c r="I17" s="9">
         <v>0</v>
       </c>
@@ -3498,16 +3568,22 @@
       <c r="L17" s="9">
         <v>0</v>
       </c>
-      <c r="M17" s="38"/>
+      <c r="M17" s="9">
+        <v>0</v>
+      </c>
       <c r="N17" s="9">
         <v>0</v>
       </c>
-      <c r="O17" s="9"/>
-      <c r="P17" s="5"/>
+      <c r="O17" s="9">
+        <v>0</v>
+      </c>
+      <c r="P17" s="45">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B18" s="4">
         <v>110</v>
@@ -3552,17 +3628,23 @@
       <c r="O18" s="9">
         <v>0.9</v>
       </c>
-      <c r="P18" s="5" t="s">
-        <v>64</v>
+      <c r="P18" s="46" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
+        <v>41</v>
+      </c>
+      <c r="B19" s="4">
+        <v>0</v>
+      </c>
+      <c r="C19" s="9">
+        <v>0</v>
+      </c>
+      <c r="D19" s="9">
+        <v>0</v>
+      </c>
       <c r="E19" s="9">
         <v>1</v>
       </c>
@@ -3572,7 +3654,9 @@
       <c r="G19" s="9">
         <v>0</v>
       </c>
-      <c r="H19" s="41"/>
+      <c r="H19" s="9">
+        <v>0</v>
+      </c>
       <c r="I19" s="9">
         <v>0</v>
       </c>
@@ -3586,20 +3670,32 @@
       <c r="L19" s="9">
         <v>0</v>
       </c>
-      <c r="M19" s="38"/>
+      <c r="M19" s="9">
+        <v>0</v>
+      </c>
       <c r="N19" s="9">
         <v>0</v>
       </c>
-      <c r="O19" s="9"/>
-      <c r="P19" s="5"/>
+      <c r="O19" s="9">
+        <v>0</v>
+      </c>
+      <c r="P19" s="45">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
+        <v>42</v>
+      </c>
+      <c r="B20" s="4">
+        <v>0</v>
+      </c>
+      <c r="C20" s="9">
+        <v>0</v>
+      </c>
+      <c r="D20" s="9">
+        <v>0</v>
+      </c>
       <c r="E20" s="9">
         <v>1</v>
       </c>
@@ -3609,7 +3705,9 @@
       <c r="G20" s="9">
         <v>0</v>
       </c>
-      <c r="H20" s="41"/>
+      <c r="H20" s="9">
+        <v>0</v>
+      </c>
       <c r="I20" s="9">
         <v>0</v>
       </c>
@@ -3623,20 +3721,32 @@
       <c r="L20" s="9">
         <v>0</v>
       </c>
-      <c r="M20" s="38"/>
+      <c r="M20" s="9">
+        <v>0</v>
+      </c>
       <c r="N20" s="9">
         <v>0</v>
       </c>
-      <c r="O20" s="9"/>
-      <c r="P20" s="5"/>
+      <c r="O20" s="9">
+        <v>0</v>
+      </c>
+      <c r="P20" s="45">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
+        <v>43</v>
+      </c>
+      <c r="B21" s="4">
+        <v>0</v>
+      </c>
+      <c r="C21" s="9">
+        <v>0</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0</v>
+      </c>
       <c r="E21" s="9">
         <v>1</v>
       </c>
@@ -3646,7 +3756,9 @@
       <c r="G21" s="9">
         <v>0</v>
       </c>
-      <c r="H21" s="41"/>
+      <c r="H21" s="9">
+        <v>0</v>
+      </c>
       <c r="I21" s="9">
         <v>0</v>
       </c>
@@ -3660,12 +3772,18 @@
       <c r="L21" s="9">
         <v>0</v>
       </c>
-      <c r="M21" s="38"/>
+      <c r="M21" s="9">
+        <v>0</v>
+      </c>
       <c r="N21" s="9">
         <v>0</v>
       </c>
-      <c r="O21" s="9"/>
-      <c r="P21" s="5"/>
+      <c r="O21" s="9">
+        <v>0</v>
+      </c>
+      <c r="P21" s="45">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>

</xml_diff>

<commit_message>
modification formules et valeurs excel
</commit_message>
<xml_diff>
--- a/Masses astres.xlsx
+++ b/Masses astres.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mael2\Desktop\Git\Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\plmie\iCloudDrive\Documents\ELISA_4\Projet_Python\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B522A1C-7A4B-4447-A0D9-EFC2CB1FEDC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103901E2-174D-4116-8DA9-CCE875F56E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="70">
   <si>
     <t>Astres</t>
   </si>
@@ -87,9 +87,6 @@
     <t>coef reduc</t>
   </si>
   <si>
-    <t>vitesse rotation équateur (rad/ds)</t>
-  </si>
-  <si>
     <t>Lune</t>
   </si>
   <si>
@@ -105,12 +102,6 @@
     <t>scale</t>
   </si>
   <si>
-    <t>3.6704</t>
-  </si>
-  <si>
-    <t>3.5562</t>
-  </si>
-  <si>
     <t>position x</t>
   </si>
   <si>
@@ -177,24 +168,12 @@
     <t>Distance au soleil</t>
   </si>
   <si>
-    <t>4 900</t>
-  </si>
-  <si>
-    <t>108 000 000</t>
-  </si>
-  <si>
     <t>49 597 870</t>
   </si>
   <si>
     <t>1 430 000 000</t>
   </si>
   <si>
-    <t>2 870 000</t>
-  </si>
-  <si>
-    <t>4 504 300 000</t>
-  </si>
-  <si>
     <t>Distance planète satellite</t>
   </si>
   <si>
@@ -253,14 +232,30 @@
   </si>
   <si>
     <t>assets/textures/dione</t>
+  </si>
+  <si>
+    <t>Diamètre (km)</t>
+  </si>
+  <si>
+    <t>Période de rotation (Jour terrestre)</t>
+  </si>
+  <si>
+    <t>Période de révolution (Jour terrestre</t>
+  </si>
+  <si>
+    <t>vitesse rotation équateur (km/jour terrestre)</t>
+  </si>
+  <si>
+    <t>vitesse rotation équateur (rad/Jour terrestre)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -335,7 +330,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -360,8 +355,14 @@
         <bgColor rgb="FFDDEBF7"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDEBF7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -502,13 +503,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF9BC2E6"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF9BC2E6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF9BC2E6"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -643,6 +672,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -650,7 +709,87 @@
     <cellStyle name="Milliers" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="47">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1047,27 +1186,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1187,20 +1305,6 @@
           <color indexed="64"/>
         </right>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1406,74 +1510,78 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{524A4480-6DAB-4CB9-8F9A-6D7582E76A58}" name="Tableau2" displayName="Tableau2" ref="A1:J21" totalsRowShown="0" headerRowDxfId="44" dataDxfId="42" headerRowBorderDxfId="43" tableBorderDxfId="41">
-  <autoFilter ref="A1:J21" xr:uid="{524A4480-6DAB-4CB9-8F9A-6D7582E76A58}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{A3C56C48-4D56-4E78-8EAC-8A8834CCB7B6}" name="Astres" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{0ACD23B6-9D0A-41BC-9D2A-22A123127B9A}" name="Masse" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{524A4480-6DAB-4CB9-8F9A-6D7582E76A58}" name="Tableau2" displayName="Tableau2" ref="A1:L21" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43">
+  <autoFilter ref="A1:L21" xr:uid="{524A4480-6DAB-4CB9-8F9A-6D7582E76A58}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{A3C56C48-4D56-4E78-8EAC-8A8834CCB7B6}" name="Astres" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{0ACD23B6-9D0A-41BC-9D2A-22A123127B9A}" name="Masse" dataDxfId="41">
       <calculatedColumnFormula>1.988*10^30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{5449565D-8FF5-4D07-BC9E-A81B7DCC7C09}" name="Diamètre" dataDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{2859AEC0-DB80-4F8A-8611-2D1CB99408B1}" name="Aplatissement" dataDxfId="37">
+    <tableColumn id="3" xr3:uid="{5449565D-8FF5-4D07-BC9E-A81B7DCC7C09}" name="Diamètre (km)" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{2859AEC0-DB80-4F8A-8611-2D1CB99408B1}" name="Aplatissement" dataDxfId="39">
       <calculatedColumnFormula>9*10^-6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{FEFB98A5-F681-4A28-8656-83E81E4A53E3}" name="Angle de rotation (deg)" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{F49A900E-B0EE-48B7-858F-35EC2942B732}" name="vitesse rotation équateur (km/h)" dataDxfId="35">
+    <tableColumn id="6" xr3:uid="{FEFB98A5-F681-4A28-8656-83E81E4A53E3}" name="Angle de rotation (deg)" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{F49A900E-B0EE-48B7-858F-35EC2942B732}" name="vitesse rotation équateur (km/jour terrestre)" dataDxfId="37">
       <calculatedColumnFormula>24*24*60*60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{7B87A2BE-ADED-4EC7-90F4-82312C153D69}" name="vitesse rotation équateur (rad/ds)" dataDxfId="34">
+    <tableColumn id="7" xr3:uid="{7B87A2BE-ADED-4EC7-90F4-82312C153D69}" name="vitesse rotation équateur (rad/Jour terrestre)" dataDxfId="36">
       <calculatedColumnFormula>DEGREES((F2*1000/3600)/(C2*1000/2))/10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{2C9717ED-55F0-43A9-8BF0-C1A01A73941C}" name="Distance au soleil" dataDxfId="33"/>
-    <tableColumn id="9" xr3:uid="{8BA55CA0-627D-44EB-B07B-B27C2C506AD3}" name="Distance planète-satellite" dataDxfId="32"/>
-    <tableColumn id="10" xr3:uid="{8E2EBB81-110D-4D53-8EB8-4CFC858D462C}" name="Temps de rotation sur elle-même" dataDxfId="31"/>
+    <tableColumn id="8" xr3:uid="{2C9717ED-55F0-43A9-8BF0-C1A01A73941C}" name="Distance au soleil" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{8BA55CA0-627D-44EB-B07B-B27C2C506AD3}" name="Distance planète-satellite" dataDxfId="35"/>
+    <tableColumn id="10" xr3:uid="{8E2EBB81-110D-4D53-8EB8-4CFC858D462C}" name="Temps de rotation sur elle-même" dataDxfId="34"/>
+    <tableColumn id="11" xr3:uid="{46007689-E22E-408A-95A0-42C987AB8891}" name="Période de rotation (Jour terrestre)" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{CEB4B556-C34F-49FE-AE7D-1C42DB00465B}" name="Période de révolution (Jour terrestre" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6B08AFF7-E6AC-487E-A862-54025ABD7D5C}" name="Tableau24" displayName="Tableau24" ref="A25:G45" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6B08AFF7-E6AC-487E-A862-54025ABD7D5C}" name="Tableau24" displayName="Tableau24" ref="A25:G45" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30">
   <autoFilter ref="A25:G45" xr:uid="{6B08AFF7-E6AC-487E-A862-54025ABD7D5C}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{57D8D285-6390-4ADD-8C08-C6E8212288A7}" name="Astres" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{9AA0953F-EB7A-4A32-8A2C-59A3B7D54DD6}" name="Masse" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{42C928A3-CDC0-401D-BBEB-DBDE9C296C9E}" name="Diamètre" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{F3774F47-11B7-41CC-BD67-B0851461EE8E}" name="Aplatissement" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{B4AE3617-38DD-4C16-A173-5946879F54C9}" name="Distance soleil" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{C1001996-59B6-404E-967B-839EFC3F25BB}" name="vitesse rotation équateur (km/h)" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{126EF6A9-B272-4BB1-AC3A-3BAF656E5D0E}" name="Distance planète satellite" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{57D8D285-6390-4ADD-8C08-C6E8212288A7}" name="Astres" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{9AA0953F-EB7A-4A32-8A2C-59A3B7D54DD6}" name="Masse" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{42C928A3-CDC0-401D-BBEB-DBDE9C296C9E}" name="Diamètre" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{F3774F47-11B7-41CC-BD67-B0851461EE8E}" name="Aplatissement" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{B4AE3617-38DD-4C16-A173-5946879F54C9}" name="Distance soleil" dataDxfId="3">
+      <calculatedColumnFormula>H2*$C$23</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{C1001996-59B6-404E-967B-839EFC3F25BB}" name="vitesse rotation équateur (km/h)" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{126EF6A9-B272-4BB1-AC3A-3BAF656E5D0E}" name="Distance planète satellite" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CE3AC303-40F0-41E2-BA80-E1255A59C86D}" name="Tableau242" displayName="Tableau242" ref="A1:P21" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CE3AC303-40F0-41E2-BA80-E1255A59C86D}" name="Tableau242" displayName="Tableau242" ref="A1:P21" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20">
   <autoFilter ref="A1:P21" xr:uid="{CE3AC303-40F0-41E2-BA80-E1255A59C86D}"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{EDE95679-AC5E-459B-B3E8-463BBC0A2BCF}" name="Astres" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{1543D1AE-2916-4C13-B130-4C9C188F65FA}" name="position x" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{BDE35151-E2B7-4D06-8610-409F0E9CE7A8}" name="position y" dataDxfId="13"/>
-    <tableColumn id="10" xr3:uid="{66091E47-CC13-44CA-922F-02228188114E}" name="position z" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{A0A9109F-3A5E-4113-B0C4-45A17BDE5075}" name="orbit speed x (m/s)" dataDxfId="11">
+    <tableColumn id="1" xr3:uid="{EDE95679-AC5E-459B-B3E8-463BBC0A2BCF}" name="Astres" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{1543D1AE-2916-4C13-B130-4C9C188F65FA}" name="position x" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{BDE35151-E2B7-4D06-8610-409F0E9CE7A8}" name="position y" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{66091E47-CC13-44CA-922F-02228188114E}" name="position z" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{A0A9109F-3A5E-4113-B0C4-45A17BDE5075}" name="orbit speed x (m/s)" dataDxfId="15">
       <calculatedColumnFormula>360/365</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{1FB021ED-D2AE-4B20-9894-A1A7B535AF42}" name="Orbit speed y" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{6447372A-4624-4464-9007-45A417812819}" name="Orbit speed z" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{BEAF4F8A-6F7B-4128-8128-A05793BBD938}" name="rotation x" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{B028B5E1-AA94-4521-955D-E61AE895B0ED}" name="rotation y" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{43855469-E423-4784-A5C9-DD6167279A62}" name="rotation z" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{8F5F32B2-D8F6-44B9-956D-C5403B260C0B}" name="OrbitRadius" dataDxfId="5">
+    <tableColumn id="11" xr3:uid="{1FB021ED-D2AE-4B20-9894-A1A7B535AF42}" name="Orbit speed y" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{6447372A-4624-4464-9007-45A417812819}" name="Orbit speed z" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{BEAF4F8A-6F7B-4128-8128-A05793BBD938}" name="rotation x" dataDxfId="12"/>
+    <tableColumn id="13" xr3:uid="{B028B5E1-AA94-4521-955D-E61AE895B0ED}" name="rotation y" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{43855469-E423-4784-A5C9-DD6167279A62}" name="rotation z" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{8F5F32B2-D8F6-44B9-956D-C5403B260C0B}" name="OrbitRadius" dataDxfId="9">
       <calculatedColumnFormula>Tableau242[[#This Row],[position x]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{90418A25-9A76-4ED3-861C-BA83D4A59328}" name="rotation speed x" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{D7830255-2F24-444E-9022-19DC045D5D90}" name="rotation speed y " dataDxfId="3">
+    <tableColumn id="4" xr3:uid="{90418A25-9A76-4ED3-861C-BA83D4A59328}" name="rotation speed x" dataDxfId="8"/>
+    <tableColumn id="15" xr3:uid="{D7830255-2F24-444E-9022-19DC045D5D90}" name="rotation speed y " dataDxfId="7">
       <calculatedColumnFormula>-360/24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{A8BA6684-B306-497B-A744-8A1D3880FB82}" name="rotation speed z" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{D0B2E9DF-29DF-408C-8213-3AD64854BC13}" name="scale" dataDxfId="1"/>
-    <tableColumn id="16" xr3:uid="{511C8A8E-79AC-4372-A019-C8C95FAF13DF}" name="Texture" dataDxfId="0"/>
+    <tableColumn id="14" xr3:uid="{A8BA6684-B306-497B-A744-8A1D3880FB82}" name="rotation speed z" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{D0B2E9DF-29DF-408C-8213-3AD64854BC13}" name="scale" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{511C8A8E-79AC-4372-A019-C8C95FAF13DF}" name="Texture" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1742,10 +1850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1755,14 +1863,16 @@
     <col min="3" max="3" width="18.88671875" customWidth="1"/>
     <col min="4" max="4" width="18.44140625" customWidth="1"/>
     <col min="5" max="5" width="31.88671875" customWidth="1"/>
-    <col min="6" max="6" width="35.88671875" customWidth="1"/>
-    <col min="7" max="7" width="33.6640625" customWidth="1"/>
-    <col min="8" max="8" width="29" customWidth="1"/>
+    <col min="6" max="6" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29" style="44" customWidth="1"/>
     <col min="9" max="9" width="26.109375" customWidth="1"/>
     <col min="10" max="10" width="39.5546875" customWidth="1"/>
+    <col min="11" max="11" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="58.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="58.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1770,31 +1880,37 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I1" s="23" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="K1" s="52" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="52" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>3</v>
       </c>
@@ -1810,25 +1926,29 @@
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2" s="9">
-        <f xml:space="preserve">  Tableau2[[#This Row],[Diamètre]]*2*PI()/(24.47*24)</f>
-        <v>14900.033453112817</v>
+        <f xml:space="preserve">  (2*PI()/Tableau2[[#This Row],[Période de rotation (Jour terrestre)]])*(Tableau2[[#This Row],[Diamètre (km)]]/2)</f>
+        <v>162046.14159896472</v>
       </c>
       <c r="G2" s="9">
-        <f>DEGREES((F2*1000/3600)/(C2*1000/2))/10</f>
-        <v>3.4055305816646229E-5</v>
-      </c>
-      <c r="H2" s="9">
+        <f xml:space="preserve">  (2*PI()/Tableau2[[#This Row],[Période de rotation (Jour terrestre)]])</f>
+        <v>0.23271056693257727</v>
+      </c>
+      <c r="H2" s="38">
         <v>0</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K2" s="47">
+        <v>27</v>
+      </c>
+      <c r="L2" s="47"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>4</v>
       </c>
@@ -1847,21 +1967,28 @@
         <v>0.03</v>
       </c>
       <c r="F3" s="9">
-        <v>10892</v>
+        <f xml:space="preserve">  (2*PI()/Tableau2[[#This Row],[Période de rotation (Jour terrestre)]])*(Tableau2[[#This Row],[Diamètre (km)]]/2)</f>
+        <v>261.36551055287362</v>
       </c>
       <c r="G3" s="9">
-        <f t="shared" ref="G3:G10" si="2">DEGREES((F3*1000/3600)/(C3*1000/2))/10</f>
-        <v>7.1054459161246225E-3</v>
-      </c>
-      <c r="H3" s="9" t="s">
+        <f xml:space="preserve">  (2*PI()/Tableau2[[#This Row],[Période de rotation (Jour terrestre)]])</f>
+        <v>0.1071301842656366</v>
+      </c>
+      <c r="H3" s="38">
+        <v>57000000</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="I3" s="9" t="s">
-        <v>53</v>
-      </c>
       <c r="J3" s="4"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K3" s="47">
+        <v>58.65</v>
+      </c>
+      <c r="L3" s="47">
+        <v>87.96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>7</v>
       </c>
@@ -1880,21 +2007,28 @@
         <v>177.36</v>
       </c>
       <c r="F4" s="9">
-        <v>6.52</v>
+        <f xml:space="preserve">  (2*PI()/Tableau2[[#This Row],[Période de rotation (Jour terrestre)]])*(Tableau2[[#This Row],[Diamètre (km)]]/2)</f>
+        <v>156.47331732023136</v>
       </c>
       <c r="G4" s="9">
-        <f t="shared" si="2"/>
-        <v>1.7146803082705271E-6</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>47</v>
+        <f xml:space="preserve">  (2*PI()/Tableau2[[#This Row],[Période de rotation (Jour terrestre)]])</f>
+        <v>2.5855665640013112E-2</v>
+      </c>
+      <c r="H4" s="38">
+        <v>108000000</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="J4" s="4"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K4" s="47">
+        <v>243.01</v>
+      </c>
+      <c r="L4" s="47">
+        <v>224.69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>8</v>
       </c>
@@ -1914,21 +2048,28 @@
         <v>23.45</v>
       </c>
       <c r="F5" s="9">
-        <v>1674.364</v>
+        <f xml:space="preserve">  (2*PI()/Tableau2[[#This Row],[Période de rotation (Jour terrestre)]])*(Tableau2[[#This Row],[Diamètre (km)]]/2)</f>
+        <v>40075.016685578485</v>
       </c>
       <c r="G5" s="9">
-        <f t="shared" si="2"/>
-        <v>4.1780743677208288E-4</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>48</v>
+        <f xml:space="preserve">  (2*PI()/Tableau2[[#This Row],[Période de rotation (Jour terrestre)]])</f>
+        <v>6.2831853071795862</v>
+      </c>
+      <c r="H5" s="38">
+        <v>149597887.5</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="J5" s="4"/>
-    </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K5" s="47">
+        <v>1</v>
+      </c>
+      <c r="L5" s="47">
+        <v>365.25599999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>9</v>
       </c>
@@ -1947,22 +2088,30 @@
         <v>25</v>
       </c>
       <c r="F6" s="9">
-        <v>868</v>
+        <f xml:space="preserve">  (2*PI()/Tableau2[[#This Row],[Période de rotation (Jour terrestre)]])*(Tableau2[[#This Row],[Diamètre (km)]]/2)</f>
+        <v>20734.731922629111</v>
       </c>
       <c r="G6" s="9">
-        <f t="shared" si="2"/>
-        <v>4.0679178623016831E-4</v>
-      </c>
-      <c r="H6" s="9">
-        <f>226*10^6</f>
-        <v>226000000</v>
+        <f xml:space="preserve">  (2*PI()/Tableau2[[#This Row],[Période de rotation (Jour terrestre)]])</f>
+        <v>6.1056336639072768</v>
+      </c>
+      <c r="H6" s="38">
+        <f>227.944*10^6</f>
+        <v>227944000</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K6" s="47">
+        <f>(24.63)/23.934</f>
+        <v>1.0290799699172724</v>
+      </c>
+      <c r="L6" s="47">
+        <v>686.97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>10</v>
       </c>
@@ -1981,22 +2130,30 @@
         <v>1.304</v>
       </c>
       <c r="F7" s="9">
-        <v>47051</v>
+        <f xml:space="preserve">  (2*PI()/Tableau2[[#This Row],[Période de rotation (Jour terrestre)]])*(Tableau2[[#This Row],[Diamètre (km)]]/2)</f>
+        <v>1092479.6851537907</v>
       </c>
       <c r="G7" s="9">
-        <f t="shared" si="2"/>
-        <v>1.0474457600034644E-3</v>
-      </c>
-      <c r="H7" s="9">
-        <f>778.6 *10^6</f>
-        <v>778600000</v>
+        <f xml:space="preserve">  (2*PI()/Tableau2[[#This Row],[Période de rotation (Jour terrestre)]])</f>
+        <v>15.281145934563177</v>
+      </c>
+      <c r="H7" s="38">
+        <f>778.34 *10^6</f>
+        <v>778340000</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="J7" s="4"/>
-    </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K7" s="47">
+        <f>(9.841)/23.934</f>
+        <v>0.41117239074120493</v>
+      </c>
+      <c r="L7" s="47">
+        <v>4332.5889999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
@@ -2014,22 +2171,30 @@
       <c r="E8" s="33">
         <v>27</v>
       </c>
-      <c r="F8" s="10">
-        <v>34821</v>
+      <c r="F8" s="9">
+        <f xml:space="preserve">  (2*PI()/Tableau2[[#This Row],[Période de rotation (Jour terrestre)]])*(Tableau2[[#This Row],[Diamètre (km)]]/2)</f>
+        <v>363925.90969074419</v>
       </c>
       <c r="G8" s="9">
-        <f t="shared" si="2"/>
-        <v>2.237899480456666E-3</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>49</v>
+        <f xml:space="preserve">  (2*PI()/Tableau2[[#This Row],[Période de rotation (Jour terrestre)]])</f>
+        <v>14.695764403599748</v>
+      </c>
+      <c r="H8" s="38">
+        <v>1426700000</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="J8" s="4"/>
-    </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K8" s="47">
+        <f>(10.233)/23.934</f>
+        <v>0.42755076460265728</v>
+      </c>
+      <c r="L8" s="47">
+        <v>10759.23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>13</v>
       </c>
@@ -2047,22 +2212,30 @@
       <c r="E9" s="9">
         <v>98</v>
       </c>
-      <c r="F9" s="10">
-        <v>9320</v>
+      <c r="F9" s="9">
+        <f xml:space="preserve">  (2*PI()/Tableau2[[#This Row],[Période de rotation (Jour terrestre)]])*(Tableau2[[#This Row],[Diamètre (km)]]/2)</f>
+        <v>214726.66652476561</v>
       </c>
       <c r="G9" s="9">
-        <f t="shared" si="2"/>
-        <v>5.8035293619330356E-4</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>50</v>
+        <f xml:space="preserve">  (2*PI()/Tableau2[[#This Row],[Période de rotation (Jour terrestre)]])</f>
+        <v>8.4012154827953207</v>
+      </c>
+      <c r="H9" s="38">
+        <v>2870700000</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="J9" s="4"/>
-    </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K9" s="47">
+        <f>(17.9)/23.934</f>
+        <v>0.74789003091835871</v>
+      </c>
+      <c r="L9" s="47">
+        <v>30685.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
         <v>14</v>
       </c>
@@ -2080,22 +2253,30 @@
       <c r="E10" s="9">
         <v>28.32</v>
       </c>
-      <c r="F10" s="10">
-        <v>9660</v>
+      <c r="F10" s="9">
+        <f xml:space="preserve">  (2*PI()/Tableau2[[#This Row],[Période de rotation (Jour terrestre)]])*(Tableau2[[#This Row],[Diamètre (km)]]/2)</f>
+        <v>231164.11135104811</v>
       </c>
       <c r="G10" s="9">
-        <f t="shared" si="2"/>
-        <v>6.2083538615236185E-4</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>51</v>
+        <f xml:space="preserve">  (2*PI()/Tableau2[[#This Row],[Période de rotation (Jour terrestre)]])</f>
+        <v>9.3346838697725776</v>
+      </c>
+      <c r="H10" s="38">
+        <v>4498400000</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="J10" s="4"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K10" s="47">
+        <f>(16.11)/23.934</f>
+        <v>0.67310102782652292</v>
+      </c>
+      <c r="L10" s="47">
+        <v>60216.800000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
       <c r="B11" s="19"/>
       <c r="C11" s="20"/>
@@ -2103,13 +2284,15 @@
       <c r="E11" s="20"/>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
+      <c r="H11" s="40"/>
       <c r="I11" s="20"/>
       <c r="J11" s="20"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K11" s="51"/>
+      <c r="L11" s="51"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="9">
         <f>7.36*10^22</f>
@@ -2128,21 +2311,23 @@
         <v>16.7</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="H12" s="38" t="s">
+        <v>43</v>
       </c>
       <c r="I12" s="9">
         <v>384400</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+      <c r="K12" s="47"/>
+      <c r="L12" s="47"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="26" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B13" s="9">
         <f>4.8 * 10^22</f>
@@ -2153,19 +2338,19 @@
         <v>3121.6</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E13" s="9">
         <v>0.46899999999999997</v>
       </c>
       <c r="F13" s="4">
-        <f>(PI()*Tableau2[[#This Row],[Diamètre]])/85</f>
+        <f>(PI()*Tableau2[[#This Row],[Diamètre (km)]])/85</f>
         <v>115.37406620524585</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H13" s="9">
+        <v>46</v>
+      </c>
+      <c r="H13" s="38">
         <f>270*10^6</f>
         <v>270000000</v>
       </c>
@@ -2173,12 +2358,14 @@
         <v>671000</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="K13" s="47"/>
+      <c r="L13" s="47"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B14" s="9">
         <f>8.9319*10^22</f>
@@ -2189,19 +2376,19 @@
         <v>3643.2</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E14" s="9">
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="F14" s="4">
-        <f>(PI()*Tableau2[[#This Row],[Diamètre]])/42.5</f>
+        <f>(PI()*Tableau2[[#This Row],[Diamètre (km)]])/42.5</f>
         <v>269.30471424843137</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H14" s="9">
+        <v>46</v>
+      </c>
+      <c r="H14" s="38">
         <f>778*10^6</f>
         <v>778000000</v>
       </c>
@@ -2209,12 +2396,14 @@
         <v>442000</v>
       </c>
       <c r="J14" s="24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="K14" s="47"/>
+      <c r="L14" s="47"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="26" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B15" s="9">
         <f>1.2 * 10^17</f>
@@ -2222,20 +2411,22 @@
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="9" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="9"/>
       <c r="G15" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H15" s="4"/>
+        <v>46</v>
+      </c>
+      <c r="H15" s="39"/>
       <c r="I15" s="5"/>
       <c r="J15" s="4"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K15" s="47"/>
+      <c r="L15" s="47"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="27" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B16" s="9">
         <f>1.4819*10^23</f>
@@ -2243,20 +2434,22 @@
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="9" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="9"/>
       <c r="G16" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H16" s="4"/>
+        <v>46</v>
+      </c>
+      <c r="H16" s="39"/>
       <c r="I16" s="5"/>
       <c r="J16" s="4"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K16" s="47"/>
+      <c r="L16" s="47"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="28" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B17" s="9">
         <f>1.88*10^21</f>
@@ -2264,20 +2457,22 @@
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="9" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="9"/>
       <c r="G17" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H17" s="9"/>
+        <v>46</v>
+      </c>
+      <c r="H17" s="38"/>
       <c r="I17" s="5"/>
       <c r="J17" s="4"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K17" s="47"/>
+      <c r="L17" s="47"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B18" s="9">
         <f>1.096 * 10^21</f>
@@ -2288,7 +2483,7 @@
         <v>1118</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E18" s="5">
         <v>2E-3</v>
@@ -2297,21 +2492,23 @@
         <v>56.73</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
+      </c>
+      <c r="H18" s="38" t="s">
+        <v>44</v>
       </c>
       <c r="I18" s="24">
         <v>377400</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+      <c r="K18" s="47"/>
+      <c r="L18" s="47"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="28" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B19" s="11">
         <f>2.306518 * 10^21</f>
@@ -2319,20 +2516,22 @@
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="9" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="9"/>
       <c r="G19" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H19" s="9"/>
+        <v>46</v>
+      </c>
+      <c r="H19" s="38"/>
       <c r="I19" s="5"/>
       <c r="J19" s="4"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K19" s="47"/>
+      <c r="L19" s="47"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="27" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B20" s="9">
         <f>2.14 * 10^22</f>
@@ -2340,20 +2539,22 @@
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="9"/>
       <c r="G20" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H20" s="9"/>
+        <v>46</v>
+      </c>
+      <c r="H20" s="38"/>
       <c r="I20" s="5"/>
       <c r="J20" s="4"/>
-    </row>
-    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K20" s="47"/>
+      <c r="L20" s="47"/>
+    </row>
+    <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="29" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B21" s="9">
         <f>1.29*10^22</f>
@@ -2361,20 +2562,22 @@
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H21" s="9"/>
+        <v>46</v>
+      </c>
+      <c r="H21" s="38"/>
       <c r="I21" s="5"/>
       <c r="J21" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="K21" s="47"/>
+      <c r="L21" s="47"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="30"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
@@ -2382,10 +2585,10 @@
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
       <c r="G22" s="5"/>
-      <c r="H22" s="10"/>
+      <c r="H22" s="37"/>
       <c r="I22" s="5"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>15</v>
       </c>
@@ -2393,9 +2596,13 @@
         <f>C26/C2</f>
         <v>7.1803797559245308E-5</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D23">
+        <f>0.0000001</f>
+        <v>9.9999999999999995E-8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>0</v>
       </c>
@@ -2415,10 +2622,10 @@
         <v>6</v>
       </c>
       <c r="G25" s="23" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
         <v>3</v>
       </c>
@@ -2427,13 +2634,15 @@
         <v>100</v>
       </c>
       <c r="D26" s="7"/>
-      <c r="E26" s="8"/>
+      <c r="E26" s="53">
+        <v>0</v>
+      </c>
       <c r="F26" s="9"/>
       <c r="G26" s="31" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
         <v>4</v>
       </c>
@@ -2443,90 +2652,108 @@
         <v>0.35035944981058154</v>
       </c>
       <c r="D27" s="10"/>
-      <c r="E27" s="9"/>
+      <c r="E27" s="48">
+        <f>H3*$D$23+100</f>
+        <v>105.7</v>
+      </c>
       <c r="F27" s="9"/>
       <c r="G27" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="9">
-        <f t="shared" ref="C28:C33" si="3">C4*$C$23</f>
+        <f t="shared" ref="C28:C33" si="2">C4*$C$23</f>
         <v>0.8690844441380815</v>
       </c>
       <c r="D28" s="10"/>
-      <c r="E28" s="9"/>
+      <c r="E28" s="48">
+        <f t="shared" ref="E28:E34" si="3">H4*$D$23+100</f>
+        <v>110.8</v>
+      </c>
       <c r="F28" s="9"/>
       <c r="G28" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B29" s="10"/>
       <c r="C29" s="9">
+        <f t="shared" si="2"/>
+        <v>0.91594891590626437</v>
+      </c>
+      <c r="D29" s="10"/>
+      <c r="E29" s="48">
         <f t="shared" si="3"/>
-        <v>0.91594891590626437</v>
-      </c>
-      <c r="D29" s="10"/>
-      <c r="E29" s="9"/>
+        <v>114.95978875</v>
+      </c>
       <c r="F29" s="9"/>
       <c r="G29" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="9">
+        <f t="shared" si="2"/>
+        <v>0.48769139302239412</v>
+      </c>
+      <c r="D30" s="5"/>
+      <c r="E30" s="48">
         <f t="shared" si="3"/>
-        <v>0.48769139302239412</v>
-      </c>
-      <c r="D30" s="5"/>
-      <c r="E30" s="9"/>
+        <v>122.7944</v>
+      </c>
       <c r="F30" s="9"/>
       <c r="G30" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B31" s="10"/>
       <c r="C31" s="9">
+        <f t="shared" si="2"/>
+        <v>10.266794190211131</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="48">
         <f t="shared" si="3"/>
-        <v>10.266794190211131</v>
-      </c>
-      <c r="D31" s="5"/>
-      <c r="E31" s="9"/>
+        <v>177.834</v>
+      </c>
       <c r="F31" s="9"/>
       <c r="G31" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B32" s="10"/>
       <c r="C32" s="9">
+        <f t="shared" si="2"/>
+        <v>3.5562984855143016</v>
+      </c>
+      <c r="D32" s="5"/>
+      <c r="E32" s="48">
         <f t="shared" si="3"/>
-        <v>3.5562984855143016</v>
-      </c>
-      <c r="D32" s="5"/>
-      <c r="E32" s="11"/>
+        <v>242.67</v>
+      </c>
       <c r="F32" s="9"/>
       <c r="G32" s="5" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -2535,14 +2762,17 @@
       </c>
       <c r="B33" s="10"/>
       <c r="C33" s="9">
+        <f t="shared" si="2"/>
+        <v>3.6704665236335017</v>
+      </c>
+      <c r="D33" s="5"/>
+      <c r="E33" s="48">
         <f t="shared" si="3"/>
-        <v>3.6704665236335017</v>
-      </c>
-      <c r="D33" s="5"/>
-      <c r="E33" s="9"/>
+        <v>387.07</v>
+      </c>
       <c r="F33" s="9"/>
       <c r="G33" s="5" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -2555,10 +2785,13 @@
         <v>3.5562984855143016</v>
       </c>
       <c r="D34" s="5"/>
-      <c r="E34" s="9"/>
+      <c r="E34" s="48">
+        <f t="shared" si="3"/>
+        <v>549.83999999999992</v>
+      </c>
       <c r="F34" s="9"/>
       <c r="G34" s="5" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -2572,7 +2805,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B36" s="9"/>
       <c r="C36" s="4">
@@ -2586,7 +2819,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="26" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
@@ -2597,7 +2830,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="25" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
@@ -2608,7 +2841,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="26" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
@@ -2619,7 +2852,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="27" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
@@ -2630,7 +2863,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="28" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B41" s="11"/>
       <c r="C41" s="9"/>
@@ -2641,7 +2874,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="27" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B42" s="9"/>
       <c r="C42" s="11">
@@ -2655,7 +2888,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="28" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
@@ -2666,7 +2899,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="27" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
@@ -2677,7 +2910,7 @@
     </row>
     <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="29" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
@@ -2725,7 +2958,7 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2748,56 +2981,57 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="H1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="J1" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="K1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="M1" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="O1" s="16" t="s">
-        <v>21</v>
-      </c>
       <c r="P1" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="9">
+        <f>Feuil1!E26</f>
         <v>0</v>
       </c>
       <c r="C2" s="9">
@@ -2831,25 +3065,25 @@
       <c r="L2" s="9">
         <v>0</v>
       </c>
-      <c r="M2" s="38">
-        <v>3600</v>
+      <c r="M2" s="54">
+        <v>0.23271056700000001</v>
       </c>
       <c r="N2" s="9">
         <v>0</v>
       </c>
-      <c r="O2" s="9">
+      <c r="O2" s="50">
         <v>100</v>
       </c>
       <c r="P2" s="17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="9">
-        <v>60</v>
+        <v>106</v>
       </c>
       <c r="C3" s="9">
         <v>0</v>
@@ -2875,32 +3109,32 @@
       <c r="J3" s="9">
         <v>0</v>
       </c>
-      <c r="K3" s="9">
+      <c r="K3" s="49">
         <f>Tableau242[[#This Row],[position x]]</f>
-        <v>60</v>
+        <v>106</v>
       </c>
       <c r="L3" s="9">
         <v>0</v>
       </c>
-      <c r="M3" s="38">
-        <v>10.891999999999999</v>
+      <c r="M3" s="55">
+        <v>0.107130184</v>
       </c>
       <c r="N3" s="9">
         <v>0</v>
       </c>
-      <c r="O3" s="9">
+      <c r="O3" s="50">
         <v>0.35034999999999999</v>
       </c>
       <c r="P3" s="17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="9">
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="C4" s="9">
         <v>0</v>
@@ -2926,32 +3160,32 @@
       <c r="J4" s="9">
         <v>0</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="49">
         <f>Tableau242[[#This Row],[position x]]</f>
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="L4" s="9">
         <v>0</v>
       </c>
-      <c r="M4" s="38">
-        <v>6.52</v>
+      <c r="M4" s="56">
+        <v>2.5855665999999999E-2</v>
       </c>
       <c r="N4" s="9">
         <v>0</v>
       </c>
-      <c r="O4" s="9">
+      <c r="O4" s="50">
         <v>0.8609</v>
       </c>
       <c r="P4" s="17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="9">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="C5" s="9">
         <v>0</v>
@@ -2977,32 +3211,32 @@
       <c r="J5" s="9">
         <v>0</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="49">
         <f>Tableau242[[#This Row],[position x]]</f>
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="L5" s="9">
         <v>0</v>
       </c>
-      <c r="M5" s="38">
-        <v>1674.364</v>
+      <c r="M5" s="55">
+        <v>6.2831853070000001</v>
       </c>
       <c r="N5" s="9">
         <v>0</v>
       </c>
-      <c r="O5" s="9">
+      <c r="O5" s="50">
         <v>0.91090000000000004</v>
       </c>
       <c r="P5" s="17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="9">
-        <v>90</v>
+        <v>123</v>
       </c>
       <c r="C6" s="9">
         <v>0</v>
@@ -3028,32 +3262,32 @@
       <c r="J6" s="9">
         <v>0</v>
       </c>
-      <c r="K6" s="9">
+      <c r="K6" s="49">
         <f>Tableau242[[#This Row],[position x]]</f>
-        <v>90</v>
+        <v>123</v>
       </c>
       <c r="L6" s="9">
         <v>0</v>
       </c>
-      <c r="M6" s="38">
-        <v>868.22</v>
+      <c r="M6" s="56">
+        <v>6.105633664</v>
       </c>
       <c r="N6" s="9">
         <v>0</v>
       </c>
-      <c r="O6" s="9">
+      <c r="O6" s="50">
         <v>0.48759999999999998</v>
       </c>
       <c r="P6" s="17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="9">
-        <v>100</v>
+        <v>178</v>
       </c>
       <c r="C7" s="9">
         <v>0</v>
@@ -3079,32 +3313,32 @@
       <c r="J7" s="9">
         <v>0</v>
       </c>
-      <c r="K7" s="9">
+      <c r="K7" s="49">
         <f>Tableau242[[#This Row],[position x]]</f>
-        <v>100</v>
+        <v>178</v>
       </c>
       <c r="L7" s="9">
         <v>0</v>
       </c>
-      <c r="M7" s="38">
-        <v>47051</v>
+      <c r="M7" s="55">
+        <v>15.281145929999999</v>
       </c>
       <c r="N7" s="9">
         <v>0</v>
       </c>
-      <c r="O7" s="9">
+      <c r="O7" s="50">
         <v>10.2667</v>
       </c>
       <c r="P7" s="17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="9">
-        <v>110</v>
+        <v>243</v>
       </c>
       <c r="C8" s="9">
         <v>0</v>
@@ -3130,32 +3364,32 @@
       <c r="J8" s="9">
         <v>0</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K8" s="49">
         <f>Tableau242[[#This Row],[position x]]</f>
-        <v>110</v>
+        <v>243</v>
       </c>
       <c r="L8" s="9">
         <v>0</v>
       </c>
-      <c r="M8" s="38">
-        <v>34821</v>
+      <c r="M8" s="56">
+        <v>14.6957644</v>
       </c>
       <c r="N8" s="9">
         <v>0</v>
       </c>
-      <c r="O8" s="9">
+      <c r="O8" s="50">
         <v>3.5562</v>
       </c>
       <c r="P8" s="17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="9">
-        <v>120</v>
+        <v>387</v>
       </c>
       <c r="C9" s="9">
         <v>0</v>
@@ -3181,32 +3415,32 @@
       <c r="J9" s="9">
         <v>0</v>
       </c>
-      <c r="K9" s="9">
+      <c r="K9" s="49">
         <f>Tableau242[[#This Row],[position x]]</f>
-        <v>120</v>
-      </c>
-      <c r="L9" s="9">
-        <v>0</v>
+        <v>387</v>
+      </c>
+      <c r="L9" s="55">
+        <v>8.4012154829999997</v>
       </c>
       <c r="M9" s="38">
-        <v>9320</v>
+        <v>0</v>
       </c>
       <c r="N9" s="9">
         <v>0</v>
       </c>
-      <c r="O9" s="9" t="s">
-        <v>22</v>
+      <c r="O9" s="50">
+        <v>3.6703999999999999</v>
       </c>
       <c r="P9" s="17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="9">
-        <v>130</v>
+        <v>550</v>
       </c>
       <c r="C10" s="9">
         <v>0</v>
@@ -3232,24 +3466,24 @@
       <c r="J10" s="9">
         <v>0</v>
       </c>
-      <c r="K10" s="9">
+      <c r="K10" s="49">
         <f>Tableau242[[#This Row],[position x]]</f>
-        <v>130</v>
+        <v>550</v>
       </c>
       <c r="L10" s="9">
         <v>0</v>
       </c>
-      <c r="M10" s="38">
-        <v>9660</v>
+      <c r="M10" s="56">
+        <v>9.3346838699999992</v>
       </c>
       <c r="N10" s="9">
         <v>0</v>
       </c>
-      <c r="O10" s="9" t="s">
-        <v>23</v>
+      <c r="O10" s="50">
+        <v>3.5562</v>
       </c>
       <c r="P10" s="17" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
@@ -3277,7 +3511,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="9">
         <v>80</v>
@@ -3323,12 +3557,12 @@
         <v>0.02</v>
       </c>
       <c r="P12" s="17" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B13" s="9">
         <v>0</v>
@@ -3379,7 +3613,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B14" s="9">
         <v>0</v>
@@ -3430,7 +3664,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B15" s="4">
         <v>0</v>
@@ -3481,7 +3715,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B16" s="4">
         <v>0</v>
@@ -3532,7 +3766,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B17" s="4">
         <v>0</v>
@@ -3583,7 +3817,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B18" s="4">
         <v>110</v>
@@ -3629,12 +3863,12 @@
         <v>0.9</v>
       </c>
       <c r="P18" s="46" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B19" s="4">
         <v>0</v>
@@ -3685,7 +3919,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B20" s="4">
         <v>0</v>
@@ -3736,7 +3970,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B21" s="4">
         <v>0</v>
@@ -3798,8 +4032,9 @@
     <hyperlink ref="A9" r:id="rId8" xr:uid="{18B4E098-5C21-4E09-A5B1-0F3248FDE337}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
   <tableParts count="1">
-    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
base de donnees mise a jour
</commit_message>
<xml_diff>
--- a/Masses astres.xlsx
+++ b/Masses astres.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mael2\Desktop\Git\Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bc217c0b68332ccc/Bureau/python/Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B522A1C-7A4B-4447-A0D9-EFC2CB1FEDC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="6_{3BAF8AEA-6EB5-456D-A8B9-C433873B345F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4ED2C15-5180-4E7A-9C60-5B9AC8B22442}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="73">
   <si>
     <t>Astres</t>
   </si>
@@ -177,24 +177,6 @@
     <t>Distance au soleil</t>
   </si>
   <si>
-    <t>4 900</t>
-  </si>
-  <si>
-    <t>108 000 000</t>
-  </si>
-  <si>
-    <t>49 597 870</t>
-  </si>
-  <si>
-    <t>1 430 000 000</t>
-  </si>
-  <si>
-    <t>2 870 000</t>
-  </si>
-  <si>
-    <t>4 504 300 000</t>
-  </si>
-  <si>
     <t>Distance planète satellite</t>
   </si>
   <si>
@@ -207,18 +189,9 @@
     <t>Temps de rotation sur elle-même</t>
   </si>
   <si>
-    <t>2,73 jours</t>
-  </si>
-  <si>
     <t>42,5 heures</t>
   </si>
   <si>
-    <t>85 heures</t>
-  </si>
-  <si>
-    <t>600 heures</t>
-  </si>
-  <si>
     <t>rotation x</t>
   </si>
   <si>
@@ -253,6 +226,36 @@
   </si>
   <si>
     <t>assets/textures/dione</t>
+  </si>
+  <si>
+    <t>Japet</t>
+  </si>
+  <si>
+    <t>655,2 heures</t>
+  </si>
+  <si>
+    <t>85,2 heures</t>
+  </si>
+  <si>
+    <t>402,8 heures</t>
+  </si>
+  <si>
+    <t>173,3 heures</t>
+  </si>
+  <si>
+    <t>1903,2 heures</t>
+  </si>
+  <si>
+    <t>68,4 heures</t>
+  </si>
+  <si>
+    <t>108 heures</t>
+  </si>
+  <si>
+    <t>141,6 heures</t>
+  </si>
+  <si>
+    <t>153,6 heures</t>
   </si>
 </sst>
 </file>
@@ -1403,6 +1406,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1744,25 +1751,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" customWidth="1"/>
-    <col min="5" max="5" width="31.88671875" customWidth="1"/>
-    <col min="6" max="6" width="35.88671875" customWidth="1"/>
-    <col min="7" max="7" width="33.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" customWidth="1"/>
+    <col min="6" max="6" width="35.85546875" customWidth="1"/>
+    <col min="7" max="7" width="33.7109375" customWidth="1"/>
     <col min="8" max="8" width="29" customWidth="1"/>
-    <col min="9" max="9" width="26.109375" customWidth="1"/>
-    <col min="10" max="10" width="39.5546875" customWidth="1"/>
+    <col min="9" max="9" width="26.140625" customWidth="1"/>
+    <col min="10" max="10" width="39.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="58.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="58.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1788,13 +1795,13 @@
         <v>45</v>
       </c>
       <c r="I1" s="23" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>3</v>
       </c>
@@ -1824,11 +1831,11 @@
         <v>0</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J2" s="4"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>4</v>
       </c>
@@ -1853,15 +1860,15 @@
         <f t="shared" ref="G3:G10" si="2">DEGREES((F3*1000/3600)/(C3*1000/2))/10</f>
         <v>7.1054459161246225E-3</v>
       </c>
-      <c r="H3" s="9" t="s">
-        <v>46</v>
+      <c r="H3" s="9">
+        <v>58000000</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>7</v>
       </c>
@@ -1886,15 +1893,15 @@
         <f t="shared" si="2"/>
         <v>1.7146803082705271E-6</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="9">
+        <v>108000000</v>
+      </c>
+      <c r="I4" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="I4" s="9" t="s">
-        <v>53</v>
-      </c>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>8</v>
       </c>
@@ -1920,15 +1927,15 @@
         <f t="shared" si="2"/>
         <v>4.1780743677208288E-4</v>
       </c>
-      <c r="H5" s="9" t="s">
-        <v>48</v>
+      <c r="H5" s="9">
+        <v>150000000</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>9</v>
       </c>
@@ -1958,11 +1965,11 @@
         <v>226000000</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>10</v>
       </c>
@@ -1992,11 +1999,11 @@
         <v>778600000</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
@@ -2021,15 +2028,15 @@
         <f t="shared" si="2"/>
         <v>2.237899480456666E-3</v>
       </c>
-      <c r="H8" s="9" t="s">
-        <v>49</v>
+      <c r="H8" s="9">
+        <v>1430000000</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>13</v>
       </c>
@@ -2054,15 +2061,15 @@
         <f t="shared" si="2"/>
         <v>5.8035293619330356E-4</v>
       </c>
-      <c r="H9" s="9" t="s">
-        <v>50</v>
+      <c r="H9" s="9">
+        <v>2870000</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>14</v>
       </c>
@@ -2087,15 +2094,15 @@
         <f t="shared" si="2"/>
         <v>6.2083538615236185E-4</v>
       </c>
-      <c r="H10" s="9" t="s">
-        <v>51</v>
+      <c r="H10" s="9">
+        <v>4504300000</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="19"/>
       <c r="C11" s="20"/>
@@ -2107,7 +2114,7 @@
       <c r="I11" s="20"/>
       <c r="J11" s="20"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
@@ -2116,31 +2123,31 @@
         <v>7.36E+22</v>
       </c>
       <c r="C12" s="5">
-        <v>3500</v>
-      </c>
-      <c r="D12" s="5">
+        <v>3474</v>
+      </c>
+      <c r="D12" s="9">
         <v>1E-3</v>
       </c>
-      <c r="E12" s="4">
-        <v>5.0999999999999996</v>
+      <c r="E12" s="39">
+        <v>5.14</v>
       </c>
       <c r="F12" s="4">
         <v>16.7</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="H12" s="9">
+        <v>49597870</v>
       </c>
       <c r="I12" s="9">
         <v>384400</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
         <v>35</v>
       </c>
@@ -2148,35 +2155,35 @@
         <f>4.8 * 10^22</f>
         <v>4.8E+22</v>
       </c>
-      <c r="C13" s="5">
-        <f>3121.6</f>
-        <v>3121.6</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>53</v>
+      <c r="C13" s="9">
+        <f>3121</f>
+        <v>3121</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="E13" s="9">
         <v>0.46899999999999997</v>
       </c>
       <c r="F13" s="4">
         <f>(PI()*Tableau2[[#This Row],[Diamètre]])/85</f>
-        <v>115.37406620524585</v>
+        <v>115.35189025710287</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="H13" s="9">
-        <f>270*10^6</f>
-        <v>270000000</v>
+        <f>778*10^6</f>
+        <v>778000000</v>
       </c>
       <c r="I13" s="24">
-        <v>671000</v>
+        <v>670900</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>36</v>
       </c>
@@ -2184,35 +2191,35 @@
         <f>8.9319*10^22</f>
         <v>8.9319000000000013E+22</v>
       </c>
-      <c r="C14" s="5">
-        <f>3643.2</f>
-        <v>3643.2</v>
+      <c r="C14" s="9">
+        <f>3643</f>
+        <v>3643</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E14" s="9">
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="F14" s="4">
         <f>(PI()*Tableau2[[#This Row],[Diamètre]])/42.5</f>
-        <v>269.30471424843137</v>
+        <v>269.28993028300272</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="H14" s="9">
         <f>778*10^6</f>
         <v>778000000</v>
       </c>
       <c r="I14" s="9">
-        <v>442000</v>
+        <v>421800</v>
       </c>
       <c r="J14" s="24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
         <v>37</v>
       </c>
@@ -2220,20 +2227,31 @@
         <f>1.2 * 10^17</f>
         <v>1.2E+17</v>
       </c>
-      <c r="C15" s="5"/>
+      <c r="C15" s="9">
+        <v>4821</v>
+      </c>
       <c r="D15" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="E15" s="9">
+        <v>0.192</v>
+      </c>
       <c r="F15" s="9"/>
       <c r="G15" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H15" s="4"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="4"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="H15" s="9">
+        <f>778*10^6</f>
+        <v>778000000</v>
+      </c>
+      <c r="I15" s="5">
+        <v>1882700</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
         <v>38</v>
       </c>
@@ -2241,41 +2259,60 @@
         <f>1.4819*10^23</f>
         <v>1.4818999999999999E+23</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="5"/>
+      <c r="C16" s="9">
+        <v>5268</v>
+      </c>
+      <c r="D16" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="9">
+        <v>0.21</v>
+      </c>
       <c r="F16" s="9"/>
       <c r="G16" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="4"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="H16" s="9">
+        <f>778*10^6</f>
+        <v>778000000</v>
+      </c>
+      <c r="I16" s="5">
+        <v>1070400</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="B17" s="9">
         <f>1.88*10^21</f>
         <v>1.88E+21</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" s="5"/>
+      <c r="C17" s="11">
+        <v>1470</v>
+      </c>
+      <c r="D17" s="9">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="E17" s="9">
+        <v>7.4889999999999999</v>
+      </c>
       <c r="F17" s="9"/>
       <c r="G17" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H17" s="9"/>
+        <v>47</v>
+      </c>
+      <c r="H17" s="9">
+        <v>1430000000</v>
+      </c>
       <c r="I17" s="5"/>
-      <c r="J17" s="4"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J17" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
         <v>40</v>
       </c>
@@ -2284,32 +2321,31 @@
         <v>1.0960000000000001E+21</v>
       </c>
       <c r="C18" s="9">
-        <f>1118</f>
-        <v>1118</v>
+        <v>1123</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="5">
+        <v>47</v>
+      </c>
+      <c r="E18" s="41">
         <v>2E-3</v>
       </c>
       <c r="F18" s="9">
         <v>56.73</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="H18" s="9">
+        <v>1430000000</v>
       </c>
       <c r="I18" s="24">
         <v>377400</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
         <v>41</v>
       </c>
@@ -2317,20 +2353,28 @@
         <f>2.306518 * 10^21</f>
         <v>2.3065180000000001E+21</v>
       </c>
-      <c r="C19" s="5"/>
+      <c r="C19" s="9">
+        <v>1527</v>
+      </c>
       <c r="D19" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="E19" s="9">
+        <v>0.33100000000000002</v>
+      </c>
       <c r="F19" s="9"/>
       <c r="G19" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H19" s="9"/>
+        <v>47</v>
+      </c>
+      <c r="H19" s="9">
+        <v>1430000000</v>
+      </c>
       <c r="I19" s="5"/>
-      <c r="J19" s="4"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J19" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>42</v>
       </c>
@@ -2338,20 +2382,30 @@
         <f>2.14 * 10^22</f>
         <v>2.1400000000000002E+22</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20" s="5"/>
+      <c r="C20" s="9">
+        <v>2706</v>
+      </c>
+      <c r="D20" s="9">
+        <v>0</v>
+      </c>
+      <c r="E20" s="9">
+        <v>157</v>
+      </c>
       <c r="F20" s="9"/>
       <c r="G20" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H20" s="9"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="4"/>
-    </row>
-    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+      <c r="H20" s="9">
+        <v>4500000000</v>
+      </c>
+      <c r="I20" s="5">
+        <v>354800</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="29" t="s">
         <v>43</v>
       </c>
@@ -2359,22 +2413,30 @@
         <f>1.29*10^22</f>
         <v>1.2900000000000001E+22</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="9"/>
+      <c r="C21" s="9">
+        <v>2377</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="E21" s="9">
+        <v>17.088999999999999</v>
+      </c>
       <c r="F21" s="9"/>
       <c r="G21" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H21" s="9"/>
-      <c r="I21" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="H21" s="9">
+        <v>5900000000</v>
+      </c>
+      <c r="I21" s="5">
+        <v>19571</v>
+      </c>
       <c r="J21" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="30"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
@@ -2385,7 +2447,7 @@
       <c r="H22" s="10"/>
       <c r="I22" s="5"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>15</v>
       </c>
@@ -2394,8 +2456,8 @@
         <v>7.1803797559245308E-5</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>0</v>
       </c>
@@ -2415,10 +2477,10 @@
         <v>6</v>
       </c>
       <c r="G25" s="23" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>3</v>
       </c>
@@ -2430,10 +2492,10 @@
       <c r="E26" s="8"/>
       <c r="F26" s="9"/>
       <c r="G26" s="31" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>4</v>
       </c>
@@ -2446,10 +2508,10 @@
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
       <c r="G27" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>7</v>
       </c>
@@ -2462,10 +2524,10 @@
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
       <c r="G28" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>8</v>
       </c>
@@ -2478,10 +2540,10 @@
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
       <c r="G29" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>9</v>
       </c>
@@ -2494,10 +2556,10 @@
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
       <c r="G30" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>10</v>
       </c>
@@ -2510,10 +2572,10 @@
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
       <c r="G31" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>12</v>
       </c>
@@ -2526,10 +2588,10 @@
       <c r="E32" s="11"/>
       <c r="F32" s="9"/>
       <c r="G32" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>13</v>
       </c>
@@ -2542,10 +2604,10 @@
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
       <c r="G33" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>14</v>
       </c>
@@ -2558,10 +2620,10 @@
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
       <c r="G34" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="18"/>
       <c r="B35" s="22"/>
       <c r="C35" s="20"/>
@@ -2570,21 +2632,21 @@
       <c r="F35" s="20"/>
       <c r="G35" s="20"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B36" s="9"/>
       <c r="C36" s="4">
         <f>C12*C23</f>
-        <v>0.25131329145735859</v>
+        <v>0.2494463927208182</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="5"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="26" t="s">
         <v>35</v>
       </c>
@@ -2595,7 +2657,7 @@
       <c r="F37" s="8"/>
       <c r="G37" s="5"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="25" t="s">
         <v>36</v>
       </c>
@@ -2606,7 +2668,7 @@
       <c r="F38" s="9"/>
       <c r="G38" s="5"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="26" t="s">
         <v>37</v>
       </c>
@@ -2617,7 +2679,7 @@
       <c r="F39" s="9"/>
       <c r="G39" s="5"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="27" t="s">
         <v>38</v>
       </c>
@@ -2628,7 +2690,7 @@
       <c r="F40" s="9"/>
       <c r="G40" s="5"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="28" t="s">
         <v>39</v>
       </c>
@@ -2639,21 +2701,21 @@
       <c r="F41" s="9"/>
       <c r="G41" s="5"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="27" t="s">
         <v>40</v>
       </c>
       <c r="B42" s="9"/>
       <c r="C42" s="11">
         <f>C18*C23</f>
-        <v>8.0276645671236255E-2</v>
+        <v>8.0635664659032477E-2</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="9"/>
       <c r="F42" s="9"/>
       <c r="G42" s="5"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="28" t="s">
         <v>41</v>
       </c>
@@ -2664,7 +2726,7 @@
       <c r="F43" s="11"/>
       <c r="G43" s="5"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="27" t="s">
         <v>42</v>
       </c>
@@ -2675,7 +2737,7 @@
       <c r="F44" s="9"/>
       <c r="G44" s="5"/>
     </row>
-    <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="29" t="s">
         <v>43</v>
       </c>
@@ -2686,7 +2748,7 @@
       <c r="F45" s="8"/>
       <c r="G45" s="5"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B46" s="10"/>
     </row>
   </sheetData>
@@ -2724,26 +2786,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD632101-F391-4EA6-87B1-6F8AAB6666B5}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView zoomScale="101" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12:H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.109375" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" customWidth="1"/>
-    <col min="5" max="7" width="21.6640625" customWidth="1"/>
-    <col min="8" max="10" width="19.88671875" customWidth="1"/>
-    <col min="11" max="11" width="23.88671875" customWidth="1"/>
-    <col min="12" max="12" width="20.6640625" customWidth="1"/>
-    <col min="13" max="13" width="20.6640625" style="44" customWidth="1"/>
-    <col min="14" max="14" width="20.6640625" customWidth="1"/>
-    <col min="15" max="15" width="26.88671875" customWidth="1"/>
-    <col min="16" max="16" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="7" width="21.7109375" customWidth="1"/>
+    <col min="8" max="10" width="19.85546875" customWidth="1"/>
+    <col min="11" max="11" width="23.85546875" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" style="44" customWidth="1"/>
+    <col min="14" max="14" width="20.7109375" customWidth="1"/>
+    <col min="15" max="15" width="26.85546875" customWidth="1"/>
+    <col min="16" max="16" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="35" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="35" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2766,7 +2828,7 @@
         <v>28</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="I1" s="16" t="s">
         <v>29</v>
@@ -2793,7 +2855,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>3</v>
       </c>
@@ -2841,10 +2903,10 @@
         <v>100</v>
       </c>
       <c r="P2" s="17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>4</v>
       </c>
@@ -2892,10 +2954,10 @@
         <v>0.35034999999999999</v>
       </c>
       <c r="P3" s="17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>7</v>
       </c>
@@ -2943,10 +3005,10 @@
         <v>0.8609</v>
       </c>
       <c r="P4" s="17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>8</v>
       </c>
@@ -2994,10 +3056,10 @@
         <v>0.91090000000000004</v>
       </c>
       <c r="P5" s="17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>9</v>
       </c>
@@ -3045,10 +3107,10 @@
         <v>0.48759999999999998</v>
       </c>
       <c r="P6" s="17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>10</v>
       </c>
@@ -3096,10 +3158,10 @@
         <v>10.2667</v>
       </c>
       <c r="P7" s="17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
@@ -3147,10 +3209,10 @@
         <v>3.5562</v>
       </c>
       <c r="P8" s="17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>13</v>
       </c>
@@ -3198,10 +3260,10 @@
         <v>22</v>
       </c>
       <c r="P9" s="17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>14</v>
       </c>
@@ -3249,10 +3311,10 @@
         <v>23</v>
       </c>
       <c r="P10" s="17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
@@ -3275,7 +3337,7 @@
       <c r="O11" s="19"/>
       <c r="P11" s="21"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
@@ -3283,7 +3345,7 @@
         <v>80</v>
       </c>
       <c r="C12" s="9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D12" s="9">
         <v>0</v>
@@ -3323,18 +3385,18 @@
         <v>0.02</v>
       </c>
       <c r="P12" s="17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B13" s="9">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C13" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D13" s="9">
         <v>0</v>
@@ -3349,7 +3411,7 @@
         <v>0</v>
       </c>
       <c r="H13" s="9">
-        <v>0</v>
+        <v>0.46899999999999997</v>
       </c>
       <c r="I13" s="9">
         <v>0</v>
@@ -3359,7 +3421,7 @@
       </c>
       <c r="K13" s="4">
         <f>Tableau242[[#This Row],[position x]]</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L13" s="9">
         <v>0</v>
@@ -3377,15 +3439,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>36</v>
       </c>
       <c r="B14" s="9">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C14" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D14" s="9">
         <v>0</v>
@@ -3400,7 +3462,7 @@
         <v>0</v>
       </c>
       <c r="H14" s="9">
-        <v>0</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="I14" s="9">
         <v>0</v>
@@ -3410,7 +3472,7 @@
       </c>
       <c r="K14" s="9">
         <f>Tableau242[[#This Row],[position x]]</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L14" s="9">
         <v>0</v>
@@ -3428,15 +3490,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>37</v>
       </c>
       <c r="B15" s="4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C15" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D15" s="9">
         <v>0</v>
@@ -3451,7 +3513,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="9">
-        <v>0</v>
+        <v>0.192</v>
       </c>
       <c r="I15" s="9">
         <v>0</v>
@@ -3461,7 +3523,7 @@
       </c>
       <c r="K15" s="9">
         <f>Tableau242[[#This Row],[position x]]</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L15" s="9">
         <v>0</v>
@@ -3479,15 +3541,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B16" s="4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C16" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D16" s="9">
         <v>0</v>
@@ -3502,7 +3564,7 @@
         <v>0</v>
       </c>
       <c r="H16" s="9">
-        <v>0</v>
+        <v>0.21</v>
       </c>
       <c r="I16" s="9">
         <v>0</v>
@@ -3512,7 +3574,7 @@
       </c>
       <c r="K16" s="9">
         <f>Tableau242[[#This Row],[position x]]</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L16" s="9">
         <v>0</v>
@@ -3530,15 +3592,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="B17" s="4">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="C17" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D17" s="9">
         <v>0</v>
@@ -3553,7 +3615,7 @@
         <v>0</v>
       </c>
       <c r="H17" s="9">
-        <v>0</v>
+        <v>7.4889999999999999</v>
       </c>
       <c r="I17" s="9">
         <v>0</v>
@@ -3563,7 +3625,7 @@
       </c>
       <c r="K17" s="9">
         <f>Tableau242[[#This Row],[position x]]</f>
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="L17" s="9">
         <v>0</v>
@@ -3581,7 +3643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>40</v>
       </c>
@@ -3604,7 +3666,7 @@
         <v>0</v>
       </c>
       <c r="H18" s="41">
-        <v>2E-3</v>
+        <v>0.02</v>
       </c>
       <c r="I18" s="9">
         <v>0</v>
@@ -3629,18 +3691,18 @@
         <v>0.9</v>
       </c>
       <c r="P18" s="46" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>41</v>
       </c>
       <c r="B19" s="4">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="C19" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D19" s="9">
         <v>0</v>
@@ -3655,7 +3717,7 @@
         <v>0</v>
       </c>
       <c r="H19" s="9">
-        <v>0</v>
+        <v>0.33100000000000002</v>
       </c>
       <c r="I19" s="9">
         <v>0</v>
@@ -3665,7 +3727,7 @@
       </c>
       <c r="K19" s="9">
         <f>Tableau242[[#This Row],[position x]]</f>
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="L19" s="9">
         <v>0</v>
@@ -3683,15 +3745,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>42</v>
       </c>
       <c r="B20" s="4">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="C20" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D20" s="9">
         <v>0</v>
@@ -3706,7 +3768,7 @@
         <v>0</v>
       </c>
       <c r="H20" s="9">
-        <v>0</v>
+        <v>157</v>
       </c>
       <c r="I20" s="9">
         <v>0</v>
@@ -3716,7 +3778,7 @@
       </c>
       <c r="K20" s="9">
         <f>Tableau242[[#This Row],[position x]]</f>
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="L20" s="9">
         <v>0</v>
@@ -3734,12 +3796,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B21" s="4">
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="C21" s="9">
         <v>0</v>
@@ -3757,7 +3819,7 @@
         <v>0</v>
       </c>
       <c r="H21" s="9">
-        <v>0</v>
+        <v>17.088999999999999</v>
       </c>
       <c r="I21" s="9">
         <v>0</v>
@@ -3767,7 +3829,7 @@
       </c>
       <c r="K21" s="9">
         <f>Tableau242[[#This Row],[position x]]</f>
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="L21" s="9">
         <v>0</v>

</xml_diff>

<commit_message>
base de donnees mise a jour (encore)
</commit_message>
<xml_diff>
--- a/Masses astres.xlsx
+++ b/Masses astres.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bc217c0b68332ccc/Bureau/python/Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="6_{3BAF8AEA-6EB5-456D-A8B9-C433873B345F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4ED2C15-5180-4E7A-9C60-5B9AC8B22442}"/>
+  <xr:revisionPtr revIDLastSave="129" documentId="6_{3BAF8AEA-6EB5-456D-A8B9-C433873B345F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7141EEFE-9B1C-4472-87B9-9B42A39B08BE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="66">
   <si>
     <t>Astres</t>
   </si>
@@ -87,15 +87,9 @@
     <t>coef reduc</t>
   </si>
   <si>
-    <t>vitesse rotation équateur (rad/ds)</t>
-  </si>
-  <si>
     <t>Lune</t>
   </si>
   <si>
-    <t>Angle de rotation (deg)</t>
-  </si>
-  <si>
     <t>7.23</t>
   </si>
   <si>
@@ -174,24 +168,12 @@
     <t>Texture</t>
   </si>
   <si>
-    <t>Distance au soleil</t>
-  </si>
-  <si>
     <t>Distance planète satellite</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
-    <t>Distance planète-satellite</t>
-  </si>
-  <si>
-    <t>Temps de rotation sur elle-même</t>
-  </si>
-  <si>
-    <t>42,5 heures</t>
-  </si>
-  <si>
     <t>rotation x</t>
   </si>
   <si>
@@ -231,31 +213,36 @@
     <t>Japet</t>
   </si>
   <si>
-    <t>655,2 heures</t>
-  </si>
-  <si>
-    <t>85,2 heures</t>
-  </si>
-  <si>
-    <t>402,8 heures</t>
-  </si>
-  <si>
-    <t>173,3 heures</t>
-  </si>
-  <si>
-    <t>1903,2 heures</t>
-  </si>
-  <si>
-    <t>68,4 heures</t>
-  </si>
-  <si>
-    <t>108 heures</t>
-  </si>
-  <si>
-    <t>141,6 heures</t>
-  </si>
-  <si>
-    <t>153,6 heures</t>
+    <t>Temps de rotation sur elle-même
+(heures)</t>
+  </si>
+  <si>
+    <t>Distance planète-satellite
+(Km)</t>
+  </si>
+  <si>
+    <t>Distance au soleil
+(Km)</t>
+  </si>
+  <si>
+    <t>vitesse rotation équateur 
+(rad/ds)</t>
+  </si>
+  <si>
+    <t>vitesse rotation équateur 
+(Km/h)</t>
+  </si>
+  <si>
+    <t>Angle de rotation 
+(deg)</t>
+  </si>
+  <si>
+    <t>Diamètre
+(Km)</t>
+  </si>
+  <si>
+    <t>Masse
+(Kg)</t>
   </si>
 </sst>
 </file>
@@ -511,7 +498,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -646,6 +633,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1417,23 +1416,23 @@
   <autoFilter ref="A1:J21" xr:uid="{524A4480-6DAB-4CB9-8F9A-6D7582E76A58}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{A3C56C48-4D56-4E78-8EAC-8A8834CCB7B6}" name="Astres" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{0ACD23B6-9D0A-41BC-9D2A-22A123127B9A}" name="Masse" dataDxfId="39">
+    <tableColumn id="2" xr3:uid="{0ACD23B6-9D0A-41BC-9D2A-22A123127B9A}" name="Masse_x000a_(Kg)" dataDxfId="39">
       <calculatedColumnFormula>1.988*10^30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{5449565D-8FF5-4D07-BC9E-A81B7DCC7C09}" name="Diamètre" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{5449565D-8FF5-4D07-BC9E-A81B7DCC7C09}" name="Diamètre_x000a_(Km)" dataDxfId="38"/>
     <tableColumn id="5" xr3:uid="{2859AEC0-DB80-4F8A-8611-2D1CB99408B1}" name="Aplatissement" dataDxfId="37">
       <calculatedColumnFormula>9*10^-6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{FEFB98A5-F681-4A28-8656-83E81E4A53E3}" name="Angle de rotation (deg)" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{F49A900E-B0EE-48B7-858F-35EC2942B732}" name="vitesse rotation équateur (km/h)" dataDxfId="35">
+    <tableColumn id="6" xr3:uid="{FEFB98A5-F681-4A28-8656-83E81E4A53E3}" name="Angle de rotation _x000a_(deg)" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{F49A900E-B0EE-48B7-858F-35EC2942B732}" name="vitesse rotation équateur _x000a_(Km/h)" dataDxfId="35">
       <calculatedColumnFormula>24*24*60*60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{7B87A2BE-ADED-4EC7-90F4-82312C153D69}" name="vitesse rotation équateur (rad/ds)" dataDxfId="34">
+    <tableColumn id="7" xr3:uid="{7B87A2BE-ADED-4EC7-90F4-82312C153D69}" name="vitesse rotation équateur _x000a_(rad/ds)" dataDxfId="34">
       <calculatedColumnFormula>DEGREES((F2*1000/3600)/(C2*1000/2))/10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{2C9717ED-55F0-43A9-8BF0-C1A01A73941C}" name="Distance au soleil" dataDxfId="33"/>
-    <tableColumn id="9" xr3:uid="{8BA55CA0-627D-44EB-B07B-B27C2C506AD3}" name="Distance planète-satellite" dataDxfId="32"/>
-    <tableColumn id="10" xr3:uid="{8E2EBB81-110D-4D53-8EB8-4CFC858D462C}" name="Temps de rotation sur elle-même" dataDxfId="31"/>
+    <tableColumn id="8" xr3:uid="{2C9717ED-55F0-43A9-8BF0-C1A01A73941C}" name="Distance au soleil_x000a_(Km)" dataDxfId="33"/>
+    <tableColumn id="9" xr3:uid="{8BA55CA0-627D-44EB-B07B-B27C2C506AD3}" name="Distance planète-satellite_x000a_(Km)" dataDxfId="32"/>
+    <tableColumn id="10" xr3:uid="{8E2EBB81-110D-4D53-8EB8-4CFC858D462C}" name="Temps de rotation sur elle-même_x000a_(heures)" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1752,7 +1751,7 @@
   <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="J2" sqref="J2:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1773,32 +1772,32 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
+      <c r="B1" s="50" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="47" t="s">
+        <v>64</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I1" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>49</v>
+      <c r="E1" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" s="47" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1817,10 +1816,11 @@
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F2" s="9">
-        <f xml:space="preserve">  Tableau2[[#This Row],[Diamètre]]*2*PI()/(24.47*24)</f>
+        <f xml:space="preserve">  Tableau2[[#This Row],[Diamètre
+(Km)]]*2*PI()/(24.47*24)</f>
         <v>14900.033453112817</v>
       </c>
       <c r="G2" s="9">
@@ -1831,7 +1831,7 @@
         <v>0</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J2" s="4"/>
     </row>
@@ -1864,7 +1864,7 @@
         <v>58000000</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J3" s="4"/>
     </row>
@@ -1897,7 +1897,7 @@
         <v>108000000</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J4" s="4"/>
     </row>
@@ -1931,7 +1931,7 @@
         <v>150000000</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J5" s="4"/>
     </row>
@@ -1965,7 +1965,7 @@
         <v>226000000</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J6" s="4"/>
     </row>
@@ -1999,7 +1999,7 @@
         <v>778600000</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J7" s="4"/>
     </row>
@@ -2032,7 +2032,7 @@
         <v>1430000000</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J8" s="4"/>
     </row>
@@ -2065,7 +2065,7 @@
         <v>2870000</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J9" s="4"/>
     </row>
@@ -2098,7 +2098,7 @@
         <v>4504300000</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J10" s="4"/>
     </row>
@@ -2116,7 +2116,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="9">
         <f>7.36*10^22</f>
@@ -2135,7 +2135,7 @@
         <v>16.7</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H12" s="9">
         <v>49597870</v>
@@ -2143,13 +2143,13 @@
       <c r="I12" s="9">
         <v>384400</v>
       </c>
-      <c r="J12" s="4" t="s">
-        <v>64</v>
+      <c r="J12" s="4">
+        <v>655.20000000000005</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B13" s="9">
         <f>4.8 * 10^22</f>
@@ -2160,17 +2160,18 @@
         <v>3121</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E13" s="9">
         <v>0.46899999999999997</v>
       </c>
       <c r="F13" s="4">
-        <f>(PI()*Tableau2[[#This Row],[Diamètre]])/85</f>
+        <f>(PI()*Tableau2[[#This Row],[Diamètre
+(Km)]])/85</f>
         <v>115.35189025710287</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H13" s="9">
         <f>778*10^6</f>
@@ -2179,13 +2180,13 @@
       <c r="I13" s="24">
         <v>670900</v>
       </c>
-      <c r="J13" s="4" t="s">
-        <v>65</v>
+      <c r="J13" s="4">
+        <v>85.2</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B14" s="9">
         <f>8.9319*10^22</f>
@@ -2196,17 +2197,18 @@
         <v>3643</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E14" s="9">
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="F14" s="4">
-        <f>(PI()*Tableau2[[#This Row],[Diamètre]])/42.5</f>
+        <f>(PI()*Tableau2[[#This Row],[Diamètre
+(Km)]])/42.5</f>
         <v>269.28993028300272</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H14" s="9">
         <f>778*10^6</f>
@@ -2215,13 +2217,13 @@
       <c r="I14" s="9">
         <v>421800</v>
       </c>
-      <c r="J14" s="24" t="s">
-        <v>50</v>
+      <c r="J14" s="24">
+        <v>42.5</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B15" s="9">
         <f>1.2 * 10^17</f>
@@ -2231,14 +2233,14 @@
         <v>4821</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E15" s="9">
         <v>0.192</v>
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H15" s="9">
         <f>778*10^6</f>
@@ -2247,13 +2249,13 @@
       <c r="I15" s="5">
         <v>1882700</v>
       </c>
-      <c r="J15" s="4" t="s">
-        <v>66</v>
+      <c r="J15" s="4">
+        <v>402.8</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B16" s="9">
         <f>1.4819*10^23</f>
@@ -2263,14 +2265,14 @@
         <v>5268</v>
       </c>
       <c r="D16" s="41" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E16" s="9">
         <v>0.21</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H16" s="9">
         <f>778*10^6</f>
@@ -2279,13 +2281,13 @@
       <c r="I16" s="5">
         <v>1070400</v>
       </c>
-      <c r="J16" s="4" t="s">
-        <v>67</v>
+      <c r="J16" s="4">
+        <v>173.3</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B17" s="9">
         <f>1.88*10^21</f>
@@ -2302,19 +2304,21 @@
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H17" s="9">
         <v>1430000000</v>
       </c>
-      <c r="I17" s="5"/>
-      <c r="J17" s="4" t="s">
-        <v>68</v>
+      <c r="I17" s="5">
+        <v>1070000</v>
+      </c>
+      <c r="J17" s="4">
+        <v>1903.2</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B18" s="9">
         <f>1.096 * 10^21</f>
@@ -2324,7 +2328,7 @@
         <v>1123</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E18" s="41">
         <v>2E-3</v>
@@ -2333,7 +2337,7 @@
         <v>56.73</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H18" s="9">
         <v>1430000000</v>
@@ -2341,13 +2345,13 @@
       <c r="I18" s="24">
         <v>377400</v>
       </c>
-      <c r="J18" s="4" t="s">
-        <v>69</v>
+      <c r="J18" s="4">
+        <v>68.400000000000006</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B19" s="11">
         <f>2.306518 * 10^21</f>
@@ -2357,26 +2361,28 @@
         <v>1527</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E19" s="9">
         <v>0.33100000000000002</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H19" s="9">
         <v>1430000000</v>
       </c>
-      <c r="I19" s="5"/>
-      <c r="J19" s="4" t="s">
-        <v>70</v>
+      <c r="I19" s="5">
+        <v>527000</v>
+      </c>
+      <c r="J19" s="4">
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B20" s="9">
         <f>2.14 * 10^22</f>
@@ -2393,7 +2399,7 @@
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H20" s="9">
         <v>4500000000</v>
@@ -2401,13 +2407,13 @@
       <c r="I20" s="5">
         <v>354800</v>
       </c>
-      <c r="J20" s="4" t="s">
-        <v>71</v>
+      <c r="J20" s="4">
+        <v>141.6</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="29" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B21" s="9">
         <f>1.29*10^22</f>
@@ -2424,7 +2430,7 @@
       </c>
       <c r="F21" s="9"/>
       <c r="G21" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H21" s="9">
         <v>5900000000</v>
@@ -2432,8 +2438,8 @@
       <c r="I21" s="5">
         <v>19571</v>
       </c>
-      <c r="J21" s="4" t="s">
-        <v>72</v>
+      <c r="J21" s="4">
+        <v>153.6</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -2477,7 +2483,7 @@
         <v>6</v>
       </c>
       <c r="G25" s="23" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -2492,7 +2498,7 @@
       <c r="E26" s="8"/>
       <c r="F26" s="9"/>
       <c r="G26" s="31" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -2508,7 +2514,7 @@
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
       <c r="G27" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -2524,7 +2530,7 @@
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
       <c r="G28" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -2540,7 +2546,7 @@
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
       <c r="G29" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -2556,7 +2562,7 @@
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
       <c r="G30" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2572,7 +2578,7 @@
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
       <c r="G31" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -2588,7 +2594,7 @@
       <c r="E32" s="11"/>
       <c r="F32" s="9"/>
       <c r="G32" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -2604,7 +2610,7 @@
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
       <c r="G33" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -2620,7 +2626,7 @@
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
       <c r="G34" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -2634,7 +2640,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B36" s="9"/>
       <c r="C36" s="4">
@@ -2648,7 +2654,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="26" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
@@ -2659,7 +2665,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="25" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
@@ -2670,7 +2676,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="26" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
@@ -2681,7 +2687,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="27" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
@@ -2692,7 +2698,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="28" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B41" s="11"/>
       <c r="C41" s="9"/>
@@ -2703,7 +2709,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B42" s="9"/>
       <c r="C42" s="11">
@@ -2717,7 +2723,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="28" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
@@ -2728,7 +2734,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="27" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
@@ -2739,7 +2745,7 @@
     </row>
     <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="29" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
@@ -2810,49 +2816,49 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="J1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I1" s="16" t="s">
+      <c r="K1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="M1" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="O1" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -2903,7 +2909,7 @@
         <v>100</v>
       </c>
       <c r="P2" s="17" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -2954,7 +2960,7 @@
         <v>0.35034999999999999</v>
       </c>
       <c r="P3" s="17" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -3005,7 +3011,7 @@
         <v>0.8609</v>
       </c>
       <c r="P4" s="17" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -3056,7 +3062,7 @@
         <v>0.91090000000000004</v>
       </c>
       <c r="P5" s="17" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -3107,7 +3113,7 @@
         <v>0.48759999999999998</v>
       </c>
       <c r="P6" s="17" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -3158,7 +3164,7 @@
         <v>10.2667</v>
       </c>
       <c r="P7" s="17" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -3209,7 +3215,7 @@
         <v>3.5562</v>
       </c>
       <c r="P8" s="17" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -3257,10 +3263,10 @@
         <v>0</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P9" s="17" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -3308,10 +3314,10 @@
         <v>0</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="P10" s="17" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -3339,7 +3345,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="9">
         <v>80</v>
@@ -3385,12 +3391,12 @@
         <v>0.02</v>
       </c>
       <c r="P12" s="17" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B13" s="9">
         <v>100</v>
@@ -3441,7 +3447,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B14" s="9">
         <v>100</v>
@@ -3492,7 +3498,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B15" s="4">
         <v>100</v>
@@ -3543,7 +3549,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B16" s="4">
         <v>100</v>
@@ -3594,7 +3600,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B17" s="4">
         <v>110</v>
@@ -3645,7 +3651,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B18" s="4">
         <v>110</v>
@@ -3691,12 +3697,12 @@
         <v>0.9</v>
       </c>
       <c r="P18" s="46" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B19" s="4">
         <v>110</v>
@@ -3747,7 +3753,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B20" s="4">
         <v>130</v>
@@ -3798,7 +3804,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B21" s="4">
         <v>140</v>

</xml_diff>

<commit_message>
base de donnees mise a jour texture map
</commit_message>
<xml_diff>
--- a/Masses astres.xlsx
+++ b/Masses astres.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\plmie\iCloudDrive\Documents\ELISA_4\Projet_Python\Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bc217c0b68332ccc/Bureau/python/Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103901E2-174D-4116-8DA9-CCE875F56E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{103901E2-174D-4116-8DA9-CCE875F56E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FD6F221-DDAA-45B3-9430-F3ACB1E6CFCA}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="78">
   <si>
     <t>Astres</t>
   </si>
@@ -247,6 +247,30 @@
   </si>
   <si>
     <t>vitesse rotation équateur (rad/Jour terrestre)</t>
+  </si>
+  <si>
+    <t>assets/textures/triton</t>
+  </si>
+  <si>
+    <t>assets/textures/europa</t>
+  </si>
+  <si>
+    <t>assets/textures/io</t>
+  </si>
+  <si>
+    <t>assets/textures/callisto</t>
+  </si>
+  <si>
+    <t>assets/textures/ganymede</t>
+  </si>
+  <si>
+    <t>assets/textures/iapetus</t>
+  </si>
+  <si>
+    <t>assets/textures/rhea</t>
+  </si>
+  <si>
+    <t>assets/textures/pluto</t>
   </si>
 </sst>
 </file>
@@ -255,7 +279,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -537,7 +561,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -667,31 +691,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -710,86 +719,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="47">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1188,6 +1117,28 @@
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1318,6 +1269,64 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1528,60 +1537,60 @@
     <tableColumn id="7" xr3:uid="{7B87A2BE-ADED-4EC7-90F4-82312C153D69}" name="vitesse rotation équateur (rad/Jour terrestre)" dataDxfId="36">
       <calculatedColumnFormula>DEGREES((F2*1000/3600)/(C2*1000/2))/10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{2C9717ED-55F0-43A9-8BF0-C1A01A73941C}" name="Distance au soleil" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{8BA55CA0-627D-44EB-B07B-B27C2C506AD3}" name="Distance planète-satellite" dataDxfId="35"/>
-    <tableColumn id="10" xr3:uid="{8E2EBB81-110D-4D53-8EB8-4CFC858D462C}" name="Temps de rotation sur elle-même" dataDxfId="34"/>
-    <tableColumn id="11" xr3:uid="{46007689-E22E-408A-95A0-42C987AB8891}" name="Période de rotation (Jour terrestre)" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{CEB4B556-C34F-49FE-AE7D-1C42DB00465B}" name="Période de révolution (Jour terrestre" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{2C9717ED-55F0-43A9-8BF0-C1A01A73941C}" name="Distance au soleil" dataDxfId="35"/>
+    <tableColumn id="9" xr3:uid="{8BA55CA0-627D-44EB-B07B-B27C2C506AD3}" name="Distance planète-satellite" dataDxfId="34"/>
+    <tableColumn id="10" xr3:uid="{8E2EBB81-110D-4D53-8EB8-4CFC858D462C}" name="Temps de rotation sur elle-même" dataDxfId="33"/>
+    <tableColumn id="11" xr3:uid="{46007689-E22E-408A-95A0-42C987AB8891}" name="Période de rotation (Jour terrestre)" dataDxfId="32"/>
+    <tableColumn id="12" xr3:uid="{CEB4B556-C34F-49FE-AE7D-1C42DB00465B}" name="Période de révolution (Jour terrestre" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6B08AFF7-E6AC-487E-A862-54025ABD7D5C}" name="Tableau24" displayName="Tableau24" ref="A25:G45" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6B08AFF7-E6AC-487E-A862-54025ABD7D5C}" name="Tableau24" displayName="Tableau24" ref="A25:G45" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27">
   <autoFilter ref="A25:G45" xr:uid="{6B08AFF7-E6AC-487E-A862-54025ABD7D5C}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{57D8D285-6390-4ADD-8C08-C6E8212288A7}" name="Astres" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{9AA0953F-EB7A-4A32-8A2C-59A3B7D54DD6}" name="Masse" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{42C928A3-CDC0-401D-BBEB-DBDE9C296C9E}" name="Diamètre" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{F3774F47-11B7-41CC-BD67-B0851461EE8E}" name="Aplatissement" dataDxfId="26"/>
-    <tableColumn id="6" xr3:uid="{B4AE3617-38DD-4C16-A173-5946879F54C9}" name="Distance soleil" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{57D8D285-6390-4ADD-8C08-C6E8212288A7}" name="Astres" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{9AA0953F-EB7A-4A32-8A2C-59A3B7D54DD6}" name="Masse" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{42C928A3-CDC0-401D-BBEB-DBDE9C296C9E}" name="Diamètre" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{F3774F47-11B7-41CC-BD67-B0851461EE8E}" name="Aplatissement" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{B4AE3617-38DD-4C16-A173-5946879F54C9}" name="Distance soleil" dataDxfId="22">
       <calculatedColumnFormula>H2*$C$23</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C1001996-59B6-404E-967B-839EFC3F25BB}" name="vitesse rotation équateur (km/h)" dataDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{126EF6A9-B272-4BB1-AC3A-3BAF656E5D0E}" name="Distance planète satellite" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{C1001996-59B6-404E-967B-839EFC3F25BB}" name="vitesse rotation équateur (km/h)" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{126EF6A9-B272-4BB1-AC3A-3BAF656E5D0E}" name="Distance planète satellite" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CE3AC303-40F0-41E2-BA80-E1255A59C86D}" name="Tableau242" displayName="Tableau242" ref="A1:P21" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CE3AC303-40F0-41E2-BA80-E1255A59C86D}" name="Tableau242" displayName="Tableau242" ref="A1:P21" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16">
   <autoFilter ref="A1:P21" xr:uid="{CE3AC303-40F0-41E2-BA80-E1255A59C86D}"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{EDE95679-AC5E-459B-B3E8-463BBC0A2BCF}" name="Astres" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{1543D1AE-2916-4C13-B130-4C9C188F65FA}" name="position x" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{BDE35151-E2B7-4D06-8610-409F0E9CE7A8}" name="position y" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{66091E47-CC13-44CA-922F-02228188114E}" name="position z" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{A0A9109F-3A5E-4113-B0C4-45A17BDE5075}" name="orbit speed x (m/s)" dataDxfId="15">
+    <tableColumn id="1" xr3:uid="{EDE95679-AC5E-459B-B3E8-463BBC0A2BCF}" name="Astres" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{1543D1AE-2916-4C13-B130-4C9C188F65FA}" name="position x" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{BDE35151-E2B7-4D06-8610-409F0E9CE7A8}" name="position y" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{66091E47-CC13-44CA-922F-02228188114E}" name="position z" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{A0A9109F-3A5E-4113-B0C4-45A17BDE5075}" name="orbit speed x (m/s)" dataDxfId="11">
       <calculatedColumnFormula>360/365</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{1FB021ED-D2AE-4B20-9894-A1A7B535AF42}" name="Orbit speed y" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{6447372A-4624-4464-9007-45A417812819}" name="Orbit speed z" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{BEAF4F8A-6F7B-4128-8128-A05793BBD938}" name="rotation x" dataDxfId="12"/>
-    <tableColumn id="13" xr3:uid="{B028B5E1-AA94-4521-955D-E61AE895B0ED}" name="rotation y" dataDxfId="11"/>
-    <tableColumn id="12" xr3:uid="{43855469-E423-4784-A5C9-DD6167279A62}" name="rotation z" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{8F5F32B2-D8F6-44B9-956D-C5403B260C0B}" name="OrbitRadius" dataDxfId="9">
+    <tableColumn id="11" xr3:uid="{1FB021ED-D2AE-4B20-9894-A1A7B535AF42}" name="Orbit speed y" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{6447372A-4624-4464-9007-45A417812819}" name="Orbit speed z" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{BEAF4F8A-6F7B-4128-8128-A05793BBD938}" name="rotation x" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{B028B5E1-AA94-4521-955D-E61AE895B0ED}" name="rotation y" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{43855469-E423-4784-A5C9-DD6167279A62}" name="rotation z" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{8F5F32B2-D8F6-44B9-956D-C5403B260C0B}" name="OrbitRadius" dataDxfId="5">
       <calculatedColumnFormula>Tableau242[[#This Row],[position x]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{90418A25-9A76-4ED3-861C-BA83D4A59328}" name="rotation speed x" dataDxfId="8"/>
-    <tableColumn id="15" xr3:uid="{D7830255-2F24-444E-9022-19DC045D5D90}" name="rotation speed y " dataDxfId="7">
+    <tableColumn id="4" xr3:uid="{90418A25-9A76-4ED3-861C-BA83D4A59328}" name="rotation speed x" dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{D7830255-2F24-444E-9022-19DC045D5D90}" name="rotation speed y " dataDxfId="3">
       <calculatedColumnFormula>-360/24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{A8BA6684-B306-497B-A744-8A1D3880FB82}" name="rotation speed z" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{D0B2E9DF-29DF-408C-8213-3AD64854BC13}" name="scale" dataDxfId="5"/>
-    <tableColumn id="16" xr3:uid="{511C8A8E-79AC-4372-A019-C8C95FAF13DF}" name="Texture" dataDxfId="4"/>
+    <tableColumn id="14" xr3:uid="{A8BA6684-B306-497B-A744-8A1D3880FB82}" name="rotation speed z" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{D0B2E9DF-29DF-408C-8213-3AD64854BC13}" name="scale" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{511C8A8E-79AC-4372-A019-C8C95FAF13DF}" name="Texture" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1852,27 +1861,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G10"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" customWidth="1"/>
-    <col min="5" max="5" width="31.88671875" customWidth="1"/>
-    <col min="6" max="6" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" customWidth="1"/>
+    <col min="6" max="6" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="29" style="44" customWidth="1"/>
-    <col min="9" max="9" width="26.109375" customWidth="1"/>
-    <col min="10" max="10" width="39.5546875" customWidth="1"/>
-    <col min="11" max="11" width="34.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="36.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.140625" customWidth="1"/>
+    <col min="10" max="10" width="39.5703125" customWidth="1"/>
+    <col min="11" max="11" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="58.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="58.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1903,14 +1912,14 @@
       <c r="J1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="52" t="s">
+      <c r="K1" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="L1" s="52" t="s">
+      <c r="L1" s="23" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>3</v>
       </c>
@@ -1943,12 +1952,12 @@
         <v>46</v>
       </c>
       <c r="J2" s="4"/>
-      <c r="K2" s="47">
+      <c r="K2" s="4">
         <v>27</v>
       </c>
-      <c r="L2" s="47"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L2" s="4"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>4</v>
       </c>
@@ -1981,14 +1990,14 @@
         <v>46</v>
       </c>
       <c r="J3" s="4"/>
-      <c r="K3" s="47">
+      <c r="K3" s="4">
         <v>58.65</v>
       </c>
-      <c r="L3" s="47">
+      <c r="L3" s="4">
         <v>87.96</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>7</v>
       </c>
@@ -2021,14 +2030,14 @@
         <v>46</v>
       </c>
       <c r="J4" s="4"/>
-      <c r="K4" s="47">
+      <c r="K4" s="4">
         <v>243.01</v>
       </c>
-      <c r="L4" s="47">
+      <c r="L4" s="4">
         <v>224.69</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>8</v>
       </c>
@@ -2062,14 +2071,14 @@
         <v>46</v>
       </c>
       <c r="J5" s="4"/>
-      <c r="K5" s="47">
+      <c r="K5" s="4">
         <v>1</v>
       </c>
-      <c r="L5" s="47">
+      <c r="L5" s="4">
         <v>365.25599999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>9</v>
       </c>
@@ -2103,15 +2112,15 @@
         <v>46</v>
       </c>
       <c r="J6" s="4"/>
-      <c r="K6" s="47">
+      <c r="K6" s="4">
         <f>(24.63)/23.934</f>
         <v>1.0290799699172724</v>
       </c>
-      <c r="L6" s="47">
+      <c r="L6" s="4">
         <v>686.97</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>10</v>
       </c>
@@ -2145,15 +2154,15 @@
         <v>46</v>
       </c>
       <c r="J7" s="4"/>
-      <c r="K7" s="47">
+      <c r="K7" s="4">
         <f>(9.841)/23.934</f>
         <v>0.41117239074120493</v>
       </c>
-      <c r="L7" s="47">
+      <c r="L7" s="4">
         <v>4332.5889999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
@@ -2186,15 +2195,15 @@
         <v>46</v>
       </c>
       <c r="J8" s="4"/>
-      <c r="K8" s="47">
+      <c r="K8" s="4">
         <f>(10.233)/23.934</f>
         <v>0.42755076460265728</v>
       </c>
-      <c r="L8" s="47">
+      <c r="L8" s="4">
         <v>10759.23</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>13</v>
       </c>
@@ -2227,15 +2236,15 @@
         <v>46</v>
       </c>
       <c r="J9" s="4"/>
-      <c r="K9" s="47">
+      <c r="K9" s="4">
         <f>(17.9)/23.934</f>
         <v>0.74789003091835871</v>
       </c>
-      <c r="L9" s="47">
+      <c r="L9" s="4">
         <v>30685.4</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>14</v>
       </c>
@@ -2268,15 +2277,15 @@
         <v>46</v>
       </c>
       <c r="J10" s="4"/>
-      <c r="K10" s="47">
+      <c r="K10" s="4">
         <f>(16.11)/23.934</f>
         <v>0.67310102782652292</v>
       </c>
-      <c r="L10" s="47">
+      <c r="L10" s="4">
         <v>60216.800000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="19"/>
       <c r="C11" s="20"/>
@@ -2287,10 +2296,10 @@
       <c r="H11" s="40"/>
       <c r="I11" s="20"/>
       <c r="J11" s="20"/>
-      <c r="K11" s="51"/>
-      <c r="L11" s="51"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>16</v>
       </c>
@@ -2322,10 +2331,10 @@
       <c r="J12" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K12" s="47"/>
-      <c r="L12" s="47"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
         <v>32</v>
       </c>
@@ -2360,10 +2369,10 @@
       <c r="J13" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="K13" s="47"/>
-      <c r="L13" s="47"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>33</v>
       </c>
@@ -2398,10 +2407,10 @@
       <c r="J14" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="K14" s="47"/>
-      <c r="L14" s="47"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
         <v>34</v>
       </c>
@@ -2421,10 +2430,10 @@
       <c r="H15" s="39"/>
       <c r="I15" s="5"/>
       <c r="J15" s="4"/>
-      <c r="K15" s="47"/>
-      <c r="L15" s="47"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
         <v>35</v>
       </c>
@@ -2444,10 +2453,10 @@
       <c r="H16" s="39"/>
       <c r="I16" s="5"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="47"/>
-      <c r="L16" s="47"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
         <v>36</v>
       </c>
@@ -2467,10 +2476,10 @@
       <c r="H17" s="38"/>
       <c r="I17" s="5"/>
       <c r="J17" s="4"/>
-      <c r="K17" s="47"/>
-      <c r="L17" s="47"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
         <v>37</v>
       </c>
@@ -2503,10 +2512,10 @@
       <c r="J18" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="K18" s="47"/>
-      <c r="L18" s="47"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
         <v>38</v>
       </c>
@@ -2526,10 +2535,10 @@
       <c r="H19" s="38"/>
       <c r="I19" s="5"/>
       <c r="J19" s="4"/>
-      <c r="K19" s="47"/>
-      <c r="L19" s="47"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>39</v>
       </c>
@@ -2549,10 +2558,10 @@
       <c r="H20" s="38"/>
       <c r="I20" s="5"/>
       <c r="J20" s="4"/>
-      <c r="K20" s="47"/>
-      <c r="L20" s="47"/>
-    </row>
-    <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="29" t="s">
         <v>40</v>
       </c>
@@ -2574,10 +2583,10 @@
       <c r="J21" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="K21" s="47"/>
-      <c r="L21" s="47"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="30"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
@@ -2588,7 +2597,7 @@
       <c r="H22" s="37"/>
       <c r="I22" s="5"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>15</v>
       </c>
@@ -2601,8 +2610,8 @@
         <v>9.9999999999999995E-8</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>0</v>
       </c>
@@ -2625,7 +2634,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>3</v>
       </c>
@@ -2634,7 +2643,7 @@
         <v>100</v>
       </c>
       <c r="D26" s="7"/>
-      <c r="E26" s="53">
+      <c r="E26" s="48">
         <v>0</v>
       </c>
       <c r="F26" s="9"/>
@@ -2642,7 +2651,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>4</v>
       </c>
@@ -2652,7 +2661,7 @@
         <v>0.35035944981058154</v>
       </c>
       <c r="D27" s="10"/>
-      <c r="E27" s="48">
+      <c r="E27" s="45">
         <f>H3*$D$23+100</f>
         <v>105.7</v>
       </c>
@@ -2661,7 +2670,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>7</v>
       </c>
@@ -2671,7 +2680,7 @@
         <v>0.8690844441380815</v>
       </c>
       <c r="D28" s="10"/>
-      <c r="E28" s="48">
+      <c r="E28" s="45">
         <f t="shared" ref="E28:E34" si="3">H4*$D$23+100</f>
         <v>110.8</v>
       </c>
@@ -2680,7 +2689,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>8</v>
       </c>
@@ -2690,7 +2699,7 @@
         <v>0.91594891590626437</v>
       </c>
       <c r="D29" s="10"/>
-      <c r="E29" s="48">
+      <c r="E29" s="45">
         <f t="shared" si="3"/>
         <v>114.95978875</v>
       </c>
@@ -2699,7 +2708,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>9</v>
       </c>
@@ -2709,7 +2718,7 @@
         <v>0.48769139302239412</v>
       </c>
       <c r="D30" s="5"/>
-      <c r="E30" s="48">
+      <c r="E30" s="45">
         <f t="shared" si="3"/>
         <v>122.7944</v>
       </c>
@@ -2718,7 +2727,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>10</v>
       </c>
@@ -2728,7 +2737,7 @@
         <v>10.266794190211131</v>
       </c>
       <c r="D31" s="5"/>
-      <c r="E31" s="48">
+      <c r="E31" s="45">
         <f t="shared" si="3"/>
         <v>177.834</v>
       </c>
@@ -2737,7 +2746,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>12</v>
       </c>
@@ -2747,7 +2756,7 @@
         <v>3.5562984855143016</v>
       </c>
       <c r="D32" s="5"/>
-      <c r="E32" s="48">
+      <c r="E32" s="45">
         <f t="shared" si="3"/>
         <v>242.67</v>
       </c>
@@ -2756,7 +2765,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>13</v>
       </c>
@@ -2766,7 +2775,7 @@
         <v>3.6704665236335017</v>
       </c>
       <c r="D33" s="5"/>
-      <c r="E33" s="48">
+      <c r="E33" s="45">
         <f t="shared" si="3"/>
         <v>387.07</v>
       </c>
@@ -2775,7 +2784,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>14</v>
       </c>
@@ -2785,7 +2794,7 @@
         <v>3.5562984855143016</v>
       </c>
       <c r="D34" s="5"/>
-      <c r="E34" s="48">
+      <c r="E34" s="45">
         <f t="shared" si="3"/>
         <v>549.83999999999992</v>
       </c>
@@ -2794,7 +2803,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="18"/>
       <c r="B35" s="22"/>
       <c r="C35" s="20"/>
@@ -2803,7 +2812,7 @@
       <c r="F35" s="20"/>
       <c r="G35" s="20"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>16</v>
       </c>
@@ -2817,7 +2826,7 @@
       <c r="F36" s="4"/>
       <c r="G36" s="5"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="26" t="s">
         <v>32</v>
       </c>
@@ -2828,7 +2837,7 @@
       <c r="F37" s="8"/>
       <c r="G37" s="5"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="25" t="s">
         <v>33</v>
       </c>
@@ -2839,7 +2848,7 @@
       <c r="F38" s="9"/>
       <c r="G38" s="5"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="26" t="s">
         <v>34</v>
       </c>
@@ -2850,7 +2859,7 @@
       <c r="F39" s="9"/>
       <c r="G39" s="5"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="27" t="s">
         <v>35</v>
       </c>
@@ -2861,7 +2870,7 @@
       <c r="F40" s="9"/>
       <c r="G40" s="5"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="28" t="s">
         <v>36</v>
       </c>
@@ -2872,7 +2881,7 @@
       <c r="F41" s="9"/>
       <c r="G41" s="5"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="27" t="s">
         <v>37</v>
       </c>
@@ -2886,7 +2895,7 @@
       <c r="F42" s="9"/>
       <c r="G42" s="5"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="28" t="s">
         <v>38</v>
       </c>
@@ -2897,7 +2906,7 @@
       <c r="F43" s="11"/>
       <c r="G43" s="5"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="27" t="s">
         <v>39</v>
       </c>
@@ -2908,7 +2917,7 @@
       <c r="F44" s="9"/>
       <c r="G44" s="5"/>
     </row>
-    <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="29" t="s">
         <v>40</v>
       </c>
@@ -2919,7 +2928,7 @@
       <c r="F45" s="8"/>
       <c r="G45" s="5"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B46" s="10"/>
     </row>
   </sheetData>
@@ -2957,26 +2966,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD632101-F391-4EA6-87B1-6F8AAB6666B5}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.109375" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" customWidth="1"/>
-    <col min="5" max="7" width="21.6640625" customWidth="1"/>
-    <col min="8" max="10" width="19.88671875" customWidth="1"/>
-    <col min="11" max="11" width="23.88671875" customWidth="1"/>
-    <col min="12" max="12" width="20.6640625" customWidth="1"/>
-    <col min="13" max="13" width="20.6640625" style="44" customWidth="1"/>
-    <col min="14" max="14" width="20.6640625" customWidth="1"/>
-    <col min="15" max="15" width="26.88671875" customWidth="1"/>
-    <col min="16" max="16" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="7" width="21.7109375" customWidth="1"/>
+    <col min="8" max="10" width="19.85546875" customWidth="1"/>
+    <col min="11" max="11" width="23.85546875" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" style="44" customWidth="1"/>
+    <col min="14" max="14" width="20.7109375" customWidth="1"/>
+    <col min="15" max="15" width="26.85546875" customWidth="1"/>
+    <col min="16" max="16" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="35" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="35" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3026,7 +3035,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>3</v>
       </c>
@@ -3065,20 +3074,20 @@
       <c r="L2" s="9">
         <v>0</v>
       </c>
-      <c r="M2" s="54">
+      <c r="M2" s="49">
         <v>0.23271056700000001</v>
       </c>
       <c r="N2" s="9">
         <v>0</v>
       </c>
-      <c r="O2" s="50">
+      <c r="O2" s="47">
         <v>100</v>
       </c>
       <c r="P2" s="17" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>4</v>
       </c>
@@ -3109,27 +3118,27 @@
       <c r="J3" s="9">
         <v>0</v>
       </c>
-      <c r="K3" s="49">
+      <c r="K3" s="46">
         <f>Tableau242[[#This Row],[position x]]</f>
         <v>106</v>
       </c>
       <c r="L3" s="9">
         <v>0</v>
       </c>
-      <c r="M3" s="55">
+      <c r="M3" s="50">
         <v>0.107130184</v>
       </c>
       <c r="N3" s="9">
         <v>0</v>
       </c>
-      <c r="O3" s="50">
+      <c r="O3" s="47">
         <v>0.35034999999999999</v>
       </c>
       <c r="P3" s="17" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>7</v>
       </c>
@@ -3160,27 +3169,27 @@
       <c r="J4" s="9">
         <v>0</v>
       </c>
-      <c r="K4" s="49">
+      <c r="K4" s="46">
         <f>Tableau242[[#This Row],[position x]]</f>
         <v>111</v>
       </c>
       <c r="L4" s="9">
         <v>0</v>
       </c>
-      <c r="M4" s="56">
+      <c r="M4" s="51">
         <v>2.5855665999999999E-2</v>
       </c>
       <c r="N4" s="9">
         <v>0</v>
       </c>
-      <c r="O4" s="50">
+      <c r="O4" s="47">
         <v>0.8609</v>
       </c>
       <c r="P4" s="17" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>8</v>
       </c>
@@ -3211,27 +3220,27 @@
       <c r="J5" s="9">
         <v>0</v>
       </c>
-      <c r="K5" s="49">
+      <c r="K5" s="46">
         <f>Tableau242[[#This Row],[position x]]</f>
         <v>115</v>
       </c>
       <c r="L5" s="9">
         <v>0</v>
       </c>
-      <c r="M5" s="55">
+      <c r="M5" s="50">
         <v>6.2831853070000001</v>
       </c>
       <c r="N5" s="9">
         <v>0</v>
       </c>
-      <c r="O5" s="50">
+      <c r="O5" s="47">
         <v>0.91090000000000004</v>
       </c>
       <c r="P5" s="17" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>9</v>
       </c>
@@ -3262,27 +3271,27 @@
       <c r="J6" s="9">
         <v>0</v>
       </c>
-      <c r="K6" s="49">
+      <c r="K6" s="46">
         <f>Tableau242[[#This Row],[position x]]</f>
         <v>123</v>
       </c>
       <c r="L6" s="9">
         <v>0</v>
       </c>
-      <c r="M6" s="56">
+      <c r="M6" s="51">
         <v>6.105633664</v>
       </c>
       <c r="N6" s="9">
         <v>0</v>
       </c>
-      <c r="O6" s="50">
+      <c r="O6" s="47">
         <v>0.48759999999999998</v>
       </c>
       <c r="P6" s="17" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>10</v>
       </c>
@@ -3313,27 +3322,27 @@
       <c r="J7" s="9">
         <v>0</v>
       </c>
-      <c r="K7" s="49">
+      <c r="K7" s="46">
         <f>Tableau242[[#This Row],[position x]]</f>
         <v>178</v>
       </c>
       <c r="L7" s="9">
         <v>0</v>
       </c>
-      <c r="M7" s="55">
+      <c r="M7" s="50">
         <v>15.281145929999999</v>
       </c>
       <c r="N7" s="9">
         <v>0</v>
       </c>
-      <c r="O7" s="50">
+      <c r="O7" s="47">
         <v>10.2667</v>
       </c>
       <c r="P7" s="17" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
@@ -3364,27 +3373,27 @@
       <c r="J8" s="9">
         <v>0</v>
       </c>
-      <c r="K8" s="49">
+      <c r="K8" s="46">
         <f>Tableau242[[#This Row],[position x]]</f>
         <v>243</v>
       </c>
       <c r="L8" s="9">
         <v>0</v>
       </c>
-      <c r="M8" s="56">
+      <c r="M8" s="51">
         <v>14.6957644</v>
       </c>
       <c r="N8" s="9">
         <v>0</v>
       </c>
-      <c r="O8" s="50">
+      <c r="O8" s="47">
         <v>3.5562</v>
       </c>
       <c r="P8" s="17" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>13</v>
       </c>
@@ -3415,11 +3424,11 @@
       <c r="J9" s="9">
         <v>0</v>
       </c>
-      <c r="K9" s="49">
+      <c r="K9" s="46">
         <f>Tableau242[[#This Row],[position x]]</f>
         <v>387</v>
       </c>
-      <c r="L9" s="55">
+      <c r="L9" s="50">
         <v>8.4012154829999997</v>
       </c>
       <c r="M9" s="38">
@@ -3428,14 +3437,14 @@
       <c r="N9" s="9">
         <v>0</v>
       </c>
-      <c r="O9" s="50">
+      <c r="O9" s="47">
         <v>3.6703999999999999</v>
       </c>
       <c r="P9" s="17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>14</v>
       </c>
@@ -3466,27 +3475,27 @@
       <c r="J10" s="9">
         <v>0</v>
       </c>
-      <c r="K10" s="49">
+      <c r="K10" s="46">
         <f>Tableau242[[#This Row],[position x]]</f>
         <v>550</v>
       </c>
       <c r="L10" s="9">
         <v>0</v>
       </c>
-      <c r="M10" s="56">
+      <c r="M10" s="51">
         <v>9.3346838699999992</v>
       </c>
       <c r="N10" s="9">
         <v>0</v>
       </c>
-      <c r="O10" s="50">
+      <c r="O10" s="47">
         <v>3.5562</v>
       </c>
       <c r="P10" s="17" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
@@ -3509,7 +3518,7 @@
       <c r="O11" s="19"/>
       <c r="P11" s="21"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>16</v>
       </c>
@@ -3560,7 +3569,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>32</v>
       </c>
@@ -3607,11 +3616,11 @@
       <c r="O13" s="9">
         <v>0</v>
       </c>
-      <c r="P13" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P13" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>33</v>
       </c>
@@ -3658,11 +3667,11 @@
       <c r="O14" s="9">
         <v>0</v>
       </c>
-      <c r="P14" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P14" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>34</v>
       </c>
@@ -3709,11 +3718,11 @@
       <c r="O15" s="9">
         <v>0</v>
       </c>
-      <c r="P15" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P15" s="17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>35</v>
       </c>
@@ -3760,11 +3769,11 @@
       <c r="O16" s="9">
         <v>0</v>
       </c>
-      <c r="P16" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P16" s="17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>36</v>
       </c>
@@ -3811,11 +3820,11 @@
       <c r="O17" s="9">
         <v>0</v>
       </c>
-      <c r="P17" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P17" s="17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>37</v>
       </c>
@@ -3862,11 +3871,11 @@
       <c r="O18" s="9">
         <v>0.9</v>
       </c>
-      <c r="P18" s="46" t="s">
+      <c r="P18" s="17" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>38</v>
       </c>
@@ -3913,11 +3922,11 @@
       <c r="O19" s="9">
         <v>0</v>
       </c>
-      <c r="P19" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P19" s="17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>39</v>
       </c>
@@ -3964,11 +3973,11 @@
       <c r="O20" s="9">
         <v>0</v>
       </c>
-      <c r="P20" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P20" s="17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>40</v>
       </c>
@@ -4015,8 +4024,8 @@
       <c r="O21" s="9">
         <v>0</v>
       </c>
-      <c r="P21" s="45">
-        <v>0</v>
+      <c r="P21" s="17" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>